<commit_message>
Get daily reddit data: Tue Jul  1 08:13:21 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_06.xlsx
+++ b/data/collected_data/2025_07_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C492"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3253 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1lovxde</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Kuromi</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lovxde</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1lovw5v</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>NOTD</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h6x0wazgy7af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1lovoai</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Burning Sensation</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lovoai/burning_sensation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1louulg</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>My new vacation set, done by me</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oc5jm84xl7af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1loufpa</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>My spirited away set from a month ago. My artist painted everything by hand ❤️</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loufpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1louebr</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>My artist went and got cateye gel and learnt how to use it the night before just for me and I love it!</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dyo0kmmpg7af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1lotqbh</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>help urgently pls 😭</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lotqbh/help_urgently_pls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1lotsxt</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>My all time favourite so far</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lotsxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1lotrsr</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>My kid's grad nails</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0k7e9ptl97af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1lotqm7</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Pride nails</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4ehzci897af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1lopv95</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Frosted doughnut nails yes or no?</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lopv95</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1lopwss</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>I’m not sure if this is the place to ask, but starter press on nails that won’t ruin my real nails?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lopwss/im_not_sure_if_this_is_the_place_to_ask_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1lor5z8</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lor5z8</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1lorysc</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>can superglued charms be removed</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lorysc/can_superglued_charms_be_removed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1los65r</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Shout out to my nail tech!</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1los65r</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1losn73</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Help- even expensive polish is peeling in 12-24 hrs</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1losn73/help_even_expensive_polish_is_peeling_in_1224_hrs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1losmr3</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>First time doing nails for a friend</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zy7bx0lix6af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1lortqq</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Any ideas for a set to go with both of these outfits?</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lortqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1lorkvz</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ez4217v3n6af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1lordyf</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>do these look cute be honest</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nyq2ou7l6af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1lor9qw</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Feeling festive</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vlxvfu73k6af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1lor69f</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Year of sets on myself ( I’m not a tech )</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lor69f</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1lor0us</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Teal Cateye</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9rbr80wh6af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1lor0ko</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>A little nail art</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1n5v3vhth6af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1loqulj</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Really happy how these little flowers turned out!</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxpvh0w8g6af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1loqke9</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Press Ons</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1loqke9/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1lopqn6</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Chipping Advice</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lopqn6</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1lop3fn</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>can i fill in luminary with ibd BIAB?</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lop3fn/can_i_fill_in_luminary_with_ibd_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1lop2h2</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Summer Set</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2079lla06af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1loos9i</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>BIAB French Manicure for Fourth of July 🇺🇸</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjr7mv2ux5af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1loomf3</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>a LIL late to the monkey trend lol</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9cqc1iew5af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1loojy6</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Why do my acrylic nails look like this?!</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loojy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1loopch</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Froggy Nails</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1blpbmu4x5af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1looov3</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Pink Torties 🐢</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1looov3</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1looixp</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Ethereal Nails</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dgz5on6kv5af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1loof3b</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>My Juicy June set 💙</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loof3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1loo6mo</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Clean stiletto nails done by @sueznails in south Philly</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loo6mo</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1loo65t</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Toes and hands . I’m in love with the colours and design</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep8qr21fs5af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1loo4a2</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>finally got my nails back after almost a year without them! wanted to try a new shape and some chrome on top! feelin like a baddie again😛</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lfqixhyr5af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1lonx3d</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Advice on growing out natural nails with gel? where do i start?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lonx3d/advice_on_growing_out_natural_nails_with_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1lonrxj</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Crooked nails</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4175tkzo5af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1lonaes</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Nail tech removed acrylic nails by clipping and picking them off - is this normal (guessing not?)?</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lonaes/nail_tech_removed_acrylic_nails_by_clipping_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1lolhte</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Advice needed on new Gel-X set</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lolhte/advice_needed_on_new_gelx_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1lonhu8</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Wedding guest nails</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lonhu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1lonbwu</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>I still have simple, short nails and now they’re matte</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a743nsh4l5af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1lon0o5</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>BTArtbox press-ons!</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lon0o5</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1lom92k</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Was itching for a French but asked my girlfriend what color I should do next. She said red so I split the difference :)</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pumwwm5gc5af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1lon4s6</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Advice on nail lamps</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lon4s6/advice_on_nail_lamps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1lom8qd</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Did my nails! Been loving 90s French lately</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1vqdppdc5af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1lom18h</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>does the gap look too big between nail and cuticle? pics from same day they were done</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lom18h</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1lolydq</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Too obviously press-ons?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lolydq</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1lolpf5</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>black french tips! just got em done fresh</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/525ar74785af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1lojh5u</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Olive nails 🫒</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9jvwqxsr4af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1lolcuh</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Fresh summer set</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86dre5gi55af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1lol4mz</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>First press-ons, painted myself, with no clue of what to do. Tips and tricks pls.</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lk72dnrs35af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1lokuxl</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Summer fun</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lokuxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1lokutu</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>french tip summer</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9a7xqnat15af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1lokthd</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Disney Nails</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uokn6vqj15af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1loktg0</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>first set from a new shop!</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loktg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1lojtts</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Tips on measuring nails for custom press-on orders?</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4y5fq0kbu4af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1lojmy3</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>I've been too scared to post because I don't think I'm doing good enough as a beginner, feedback?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lojmy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1lojjwb</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>I have very hard cuticles all over my nail plate, I can't remove them even with cuticle remover :/, they make it very difficult for me to apply nail polish. What can I do?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5x5x71lcs4af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1lojc57</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Can polymer gel be used as a bond between natural nails and press ons ?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lojc57/can_polymer_gel_be_used_as_a_bond_between_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1loj9td</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>red cat eye</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0vmwyvdq4af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1loj3o2</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Help!! Tips for a newbie who wants to get them done in around 1h?</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loj3o2</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1loiyh0</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Showing off the fancy key holder and my nails 🙂</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2ckx5q4o4af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1loip9v</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>I'll probably die with glitter nails. So obsessed/addicted✨ 💕🩷✨</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3zpv6xam4af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1loguxq</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Birthday nail inspo help! (All pics found on Pinterest) https://pin.it/3iPvp6slz https://pin.it/3yb2ymGNF https://pin.it/45OyUzPRG https://pin.it/48VmUE1sT https://pin.it/6I2YpZzQV</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loguxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1lohuwj</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Favorite regular nail polish? TIA!</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lohuwj/favorite_regular_nail_polish_tia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1lohlli</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>I broke my nail.</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9p8fxs1ne4af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1lohifr</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Am I being too picky?</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lohifr</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1lohc4t</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>What did I do wrong??</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lohc4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1loh67j</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Whats on my nails??</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2gpyq19nb4af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1loh4a9</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>I have found my perfect shape after TEN YEARS of always having nails 😭</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loh4a9</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1loh212</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Luminary Builder gel lifting</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/750wnd0ua4af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1logtc4</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>My Signature Color</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9wwzat3594af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1lofxhq</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>New summer set!</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4il91ug034af1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1lofwhj</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Did my dil’s nails…</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lofwhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1lofr7c</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Last theme nail for awhile 🌭</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lofr7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1lofifw</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>New nails!!!</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lofifw</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1loet9r</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Which nails for 4th of July weekend / look best on me</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loet9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1loe220</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Vacation Ready!</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1xgjdl9q3af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1lod0hw</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Finally found „my recipe“</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vyuxpmlaj3af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1locttp</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>need you guys to laugh with me so I don’t cry</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1locttp</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1locqh5</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Three months as a nail tech :)</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5x24vphh3af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1locqcr</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Does this look good? Any recommendations?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1locqcr</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1loaywd</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Gel-X w/ bruised nail?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2zvpb6kd53af1</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1lo53fj</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>HELP! what do i ask for? (NOT MY PHOTOS: credit to @chicnailsbyAG, @themoodguide on pinterest)</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lo53fj</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1lo4pnb</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>My Drill is possessed by demons or something</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c3h3ezafr1af1</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1lockqb</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>is there such a thing as too much ✨ glitter ✨?</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lockqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1lo68cg</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Press ons?</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lo68cg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1lo7h14</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Why does my nail polish crack like this?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lo7h14</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1lochue</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Been learning hownto do my own nails at home 😊 2nd time trying, and I am super happy with them! These are my natural nails with gel polish 😊</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lochue</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1lo7s79</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>cut down all my natural nails for this 🥲</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lo7s79</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1locgm8</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Vacation nails 💅</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hg8x72mmf3af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1lob4ie</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Protect natural nail length?</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ot3d9btf63af1</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1locdhl</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>wanted something dreamy and magical</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1locdhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1loc5dh</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>4th ready! Did these myself  ⭐️🇺🇸</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/225d13zgd3af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1lobj1k</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>My fav set yet ✨</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6l3evqe693af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1lobae2</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Do press ons ruin your nails? If not, best brands?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lobae2/do_press_ons_ruin_your_nails_if_not_best_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1louzy7</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Got my Cosmic Polish order - colour me impressed!</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8oqyy2pon7af1</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1loubzo</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Urban Decay polish in Zodiac (2016)</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9uya3xxf7af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1lou6dp</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Is it possible to fix this? or something??</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lou6dp</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1losm0e</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Getting nail polish REMOVER out of clothes??</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dd20i8xax6af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1losd5m</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Electric Summer Skittle</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lojhym</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1los80h</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>When your claws match T-Rex’s… call it a Jurassic sparkle ✨✨</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1los7s3</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1loruk5</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Last day of pride month</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hehyf0nrp6af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1lorkp3</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>BKL’s I Choose the Bear</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bodbzh32n6af1</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1lorh1c</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Cupcake Swatches</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lorh1c/cupcake_swatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1lor88b</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Had to share before Pride Month is over!</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lor88b</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1loqus7</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>advice to keep my polish from chipping</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lopm83</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1loqnas</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>🩷💜💙</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loqnas</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1lopvau</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>A month of purple manis💜</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lopvau</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1lopo62</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>🩷🤍🩵</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lopo62</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1lopg2n</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Which indie brands have the easiest/hardest magnetics to work with?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lopg2n/which_indie_brands_have_the_easiesthardest/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1loowot</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>June Manicure Round Up!</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loowot</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1loou5n</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Has anyone here almost given up on neon pigments?</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1loou5n/has_anyone_here_almost_given_up_on_neon_pigments/</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1loosrz</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Can the apex change?</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwj1eyuyx5af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1loonet</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>🌈Neon✨️ for Summer🏖</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rj0c0enw5af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1loo3yn</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>ILNP Love Language</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loo3yn</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1loo1xq</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>ILNP Deep Space 🌌</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loo1xq</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1lontwq</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Indecisive so went with all of em🤣</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3iggt6ygp5af1</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1lonia2</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Since I've seen some July 4th nails...</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lazb46aom5af1</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1lond76</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Day 8 of Tyler's Trinkets Unapologetic Collection</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f86vfo9il5af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1lomzb7</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Flaky Green Polish Reccs?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lomzb7/flaky_green_polish_reccs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1lombje</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Loving this combo!</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wlglw9mzc5af1</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1lomb69</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>A very starry manicure⭐️🌙</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lomb69</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1lom1oy</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Clionadh Canada Day Flash Sale - 15% off until July 3rd</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lom1oy/clionadh_canada_day_flash_sale_15_off_until_july/</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1loleue</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>a new summer favorite</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loleue</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1lol9r2</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>dupe for alloy matey by orly?</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lol9r2/dupe_for_alloy_matey_by_orly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1lol7x5</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Lurid flakies ✨</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qw118pch45af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1lol485</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Need help healing my cuticle</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5izn9nvp35af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1lokjjh</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>June Manis 🌈</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lokjjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1lok65i</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>I know it’s not a super summery look, but I don’t care.</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lok65i</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1lok13s</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>I made a swatch book</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lok13s/i_made_a_swatch_book/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1lok0an</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>My Cliodhna collection is growing!</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ad6jilpmv4af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1lojxdg</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Atomic Polish: Redrum</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lojxdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1lojcul</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Happy birthday Canada 🇨🇦</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bntmz47zq4af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1loiymn</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Why does it seem like every time I use quick-drying top coat they remove my color?</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loiymn</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1loir5m</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>PPU and Maniology delivered today!</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qj7lr1aom4af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1loi4jn</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Cadillacquer Neon Lights</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loi4jn</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1loi1l3</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>🧜‍♀️🧜‍♂️Dreamy Mermaid vibes for a heatwave!</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loi1l3</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1lohym3</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Cracked Polish</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lohym3/cracked_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1lohwbc</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Rocking a rainbow skittle these last few days of pride</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lohwbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1lohpfd</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>I love french manicure, how can I do it easily?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lohpfd/i_love_french_manicure_how_can_i_do_it_easily/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1lohn87</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Glowy goodness on a hot summer evening…</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1xs3gzxe4af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1lohcir</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Searching for a better sheer nude</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lohcir</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1log4c9</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Help me decide!</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1log4c9</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1lofvls</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Polish Me Silly Firecracker Glow</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lofvls</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1lofpac</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Gimme some ideas for organizing!</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lofpac/gimme_some_ideas_for_organizing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1lof8hz</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Jellies that work well with the glass nails technique?</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lof8hz/jellies_that_work_well_with_the_glass_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1loelfk</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Exciting Magnetics</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1loelfk/exciting_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1lodvkb</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>BKL fans, I just posted a swatch and review of the new Tenderly I Am Devoured collection on my YouTube. Please give it a watch! 🦢</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lodvkb</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1lodtcm</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>What colors/types fade with time?</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lodtcm/what_colorstypes_fade_with_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1lodehi</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>I’m FINALLY improving my longevity!</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lodehi</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1lod7a8</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Some neutrals to start the week</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lod7a8</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1lo2oo6</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>first attempt at painting pressons for myself!</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcl3ao0o41af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1lod35x</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Fourth of July fun</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4y30uvrj3af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1lociu1</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Best glow in the dark polish?</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lociu1/best_glow_in_the_dark_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1loc4cl</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>From 2014 to 2025 - Starrily's Ultima is STILL That Girl 💅🏼</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loc4cl</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1lobv5a</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Vitamin Glow</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgd0r02ib3af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1lobu0z</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Swatch fun</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i33pwe4ab3af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1lobea7</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>i can’t tell if i like these 🤪</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lobea7</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1lob9li</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Label the stainers?</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lob9li/label_the_stainers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1loabr1</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Unsure about this combo</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loabr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1loa4oc</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>What polish did you love so much you had to go back out and buy three more?</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvcg1vrkz2af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1lo97ds</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Warm and cosy for gale force winds</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lo97ds</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1lo8zg8</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Brands other than Mooncat that donated for Pride this year?</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lo8zg8/brands_other_than_mooncat_that_donated_for_pride/</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1lo7yq0</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Bee’s Knees shipping?</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lo7yq0/bees_knees_shipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1lo72l9</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Swatches of Molten Sky and Fields of Lavender?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lo72l9/swatches_of_molten_sky_and_fields_of_lavender/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1lo3po5</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Does this swatcher edit their photos?</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lo3po5</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1lo48nu</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>So what exactly IS the difference between these two?</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lo48nu</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1lo3mfx</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lo3mfx/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1louhqd</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Acrylic Progress over 10y, 2 weeks at a time</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1louhqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1los1ov</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>fish&amp; fruit press-ons 🐟🫐</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1los1ov</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1los0ex</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1los0ex</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1lorcn3</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Ombré In July</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5cyl0i1vk6af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1loqszt</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Hot Dog 🌭 Nails</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loqszt</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1loppie</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Anybody know how I can do it my nails looks like that? 💅</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loppie</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1lopnd0</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Nail conditions nail art 💅</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9oddbjyg56af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1lopeqj</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Best gel starter kits in canada?</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lopeqj/best_gel_starter_kits_in_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1lop7to</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Our nails for friends wedding!</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lop7to</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1loodws</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>posting some nail inspo for anyone that needs it 🫡 used gel for all of these!</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loodws</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1lomhwz</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>First Nails Since Chemo!</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xrkefpffe5af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1lokza7</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Tried marble nail art recently 🍑</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6dqi0ip25af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1lohtqy</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>love a holiday themed nail</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ds02r2q7g4af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1lodnmw</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>My nail lady is amazing!</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lodnmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1lod84o</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Me gustan los tonos, pero no me quedó muy bonito el diseño !</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lod84o</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1lo946x</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Prancing in Purple🩰🕺💜</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lo946x</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1lo67fb</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Pokémon nails</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyu0wk0m52af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1lo5kv4</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Stars💗✨</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lo5kv4</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jul  2 08:13:23 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_06.xlsx
+++ b/data/collected_data/2025_07_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C492"/>
+  <dimension ref="A1:C721"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8797,6 +8797,3899 @@
         </is>
       </c>
     </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1lppmxs</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Found an amazing person who does nails from her home</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lppmxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1lpphox</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Rilakkuma press ons I made^^</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpphox</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1lpp8te</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>nail problems</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lpp8te/nail_problems/</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1lppdz6</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>my bad press ons i made</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lppdz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1lpoj7d</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Did these myself and itching to redo</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vaqhitbleaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1lpoqch</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>My lil strawbebbies all done by my partially paralyzed hands with adaptive tools 🍓</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edvediynneaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1lpoo79</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>More of my recent nails</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpoo79</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1lpofab</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Add a design on these or no?</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5u8cn23keaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1lpnxm2</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Would like some feedback</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpnxm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1lpnvnf</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Nail conditions nail art 💅</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o74amij1eeaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1lpnv2l</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>First time using press ons!!</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpnv2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1lpnt2a</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>My Nail Tech never misses 💅🏽</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpnt2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1lpkzeb</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>ISO: lotion that nail salons use</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lpkzeb/iso_lotion_that_nail_salons_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1lpn7wh</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>I just got my birthday nails!</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpn7wh</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1lp8o5m</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>I NEED nails</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1dnta86yaaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1lp1qo5</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Any advice on how to stop nails tearing so I can grow out my side walls?</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcs2ti8yl9af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1lpc0q0</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Anyone have any 3D printable nail art storage solutions?</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lpc0q0/anyone_have_any_3d_printable_nail_art_storage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1lpmx1c</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>I made nail art with art supplies!</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpmx1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1lpn1oq</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>All my favourite fruits</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvrtzvz55eaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1lpmn9r</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>My kid (25) made this spirited away themed set</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gy8i8xc31eaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1lplp6a</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Cherries for summer 🍒</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnvqkuuwrdaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1lploe5</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>no title, but...</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wegzp4wnrdaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1lpln73</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>A year of getting my nails done</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpln73</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1lpjin7</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Fancy Nancy inspired</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwn1vsmz7daf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1lpl0yk</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Not bad for my 2nd try?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpl0yk</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1lpkqzv</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Que tal quedaron?</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ccavcg4jdaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1lpk01e</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Jealous of everyone’s nails that don’t grow upward</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/agn28oq9cdaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1lpjzhg</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>My girlfriend used pimple patches as nail art</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4o7sisl4cdaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1lpjz1l</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Stripes and polka dots</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpjz1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1lpjyej</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>How much would you pay?</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpjyej</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1lpjo9j</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Paid $135 for this mani/pedi and I'm really disappointed</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpjo9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1lpjgeh</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>That one nail....</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zif55d8f7daf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1lp1ng5</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>My almond nails! I like them better this way than straight! What do you think?</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omzkixe8l9af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1lpawdt</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Brand New XL Beetlejuice-Inspired Nails!</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpawdt</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1lpfjw0</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>DIY engagement nails??</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpfjw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1lp8qbw</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>at home nail tech and cats</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lp8qbw/at_home_nail_tech_and_cats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1lotznx</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>What is this nail shape called</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lotznx/what_is_this_nail_shape_called/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1lpj94b</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>growing my nail beds</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eggd2jhm5daf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1lotuho</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Using Gel-x primer products for glue-on nails?</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lotuho/using_gelx_primer_products_for_glueon_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1lpe5y6</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>I gave myself nails based off shoes I saw on Pinterest</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpe5y6</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1lpg2kk</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>How to help these heal? Over did it with my glass cuticle pusher and my nails have never looked worse :(</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpg2kk</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1lpgn8f</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>⛓️‍💥 🚬 Telephone ⚠️ 📞</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpgn8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1lphnq7</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>How do you stop glue overflow with press-ons?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lphnq7/how_do_you_stop_glue_overflow_with_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1lpj3zb</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Still learning how to do my own</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpj3zb</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1lpeozd</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>My first real set with nail art. Inspired by my favorite anime boy, Itachi Uchiha!</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/89ejei444caf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1lpicjb</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Removing Press on Nails</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lpicjb/removing_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1lpiyrq</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>summer ice creeeam 🍨</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpiyrq</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1lpe9pd</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Gel Lamps</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lpe9pd/gel_lamps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1lphq5l</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Oranges &amp; Porcelain</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lphq5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1lpi20j</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Very obsessed.</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/537sv721vcaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1lpi0d8</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>First attempt at a cat eye, second attempt at gel 😌</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/boy6fzgnucaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1lphug6</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Bellbottom Denim makes me want to rock my favorite jeans !!</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6juuew7tcaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1lphmup</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Almond Shape?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irgb2ocgrcaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1lphavj</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Peach vibes this summer</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lphavj</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1lph82k</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Boyfriend did my fishy nails</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lph82k</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1lph362</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>I’m beginning to feel like I did this right.</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0ag84stxmcaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1lpgv3d</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>PCB airbrush tshirt</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpgv3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1lpgbwk</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>wanted to share some of my fav press ons i’ve made recently 🥹</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpgbwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1lpfz41</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>My new set.. done by me</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpfz41</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1lpekwf</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Where to buy extra slim full cover nails?</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lpekwf/where_to_buy_extra_slim_full_cover_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1lpe34v</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>New Set!</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpe34v</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1lpdo81</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>White flowers with a little cat eye polish</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ta4arffnwbaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1lpdiju</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Please give me ideas for next set</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpdiju</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1lpddus</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Opinion on Beetle gelpolish?</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lpddus/opinion_on_beetle_gelpolish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1lpcqsm</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Started doing my own press ons recently. Part 2 of a fruit series: strawberries!</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpcqsm</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1lpbymr</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Will press ons damadge my natural nails?</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lpbymr/will_press_ons_damadge_my_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1lpbng8</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>New nails, forever rainbow</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpbng8</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1lpbfwv</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Where to find these clip on nails? And if could cheaper alternatives</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lpbfwv/where_to_find_these_clip_on_nails_and_if_could/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1lpaep2</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e11cqxlw9baf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1lpaed1</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Half tips- small size recommendations</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lpaed1/half_tips_small_size_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1lpabx1</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>50 shades of pink</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0dn57bhd9baf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1lpa3sv</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Newwwww ones! what do we say?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8f3v60ww7baf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1lp98a1</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/falmq64x1baf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1lp8yme</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Hawaii Vibes 🌊🌿🍋‍🟩</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w53mrv140baf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1lp8tx2</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Off-service Nails</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3d7sq038zaaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1lp8lyt</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>seashells</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xob9wosxaaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1lp8fa4</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>which ones are cuter ? ?  i need help choosing &gt;ᴗ&lt;</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp8fa4</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1lp8ba4</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Bonito diseño uñas cortas</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0secvazpvaaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1lp8576</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>I was asked to freestyle so this is what I did for her</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6bt8x6luaaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1lp7pvh</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>my summer nails🌸🌼</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp7pvh</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1lp7nl8</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>neon yellow pedi for july @nailbeatz</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drqey01braaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1lp68ou</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>So proud with how far my natural nails have come!</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp68ou</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1lp6x9p</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>My nails!</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6p8jzxgimaaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1lp6pnf</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Press on game is gettin’ crazyyy!!!</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp6pnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1lp63qk</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Jumped on the Fruity Train</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/euhbfd2zgaaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1lp5v2i</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Asked for nails that matched my paddleboard</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp5v2i</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1lp5i4g</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>My wedding nails ♥️</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp5i4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1lp5f8j</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Best press on brands?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lp5f8j/best_press_on_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1lp55mv</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Broke a nail in Ibiza :(</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aorg0gyhaaaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1lp542k</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Super proud of these</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ev7yro7aaaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1lp5427</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>What can you say about this pair?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp5427</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1lp4r9j</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Can this be fixed!?!</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqvon0vr7aaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1lp44g7</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>When you find the perfect red for your skin tone</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp44g7</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1lp3v9l</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>LABUBU NAILS.✨</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp3v9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1lp3hhk</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>How can I make extensions that fit me using a stand?</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lp3hhk/how_can_i_make_extensions_that_fit_me_using_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1lp3gkg</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Sweet nails like a sunset on the beach🌺🐚.</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp3gkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1lp3g65</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Cigarette nails</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp3g65</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1lp3e3c</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>From Damaged to Healthy 😍</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ky826may9af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1lp2wj9</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Which nail is your favourite?</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp2wj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1lp2ven</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Ex Nail Biter - 16 weeks between today's set and my first!</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp2ven</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1lpo8fy</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>My perfect PPU Skittle + 1</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gyt220i1ieaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1lpnnb1</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Nail conditions nail art</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rar8ykjjbeaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1lpn3hw</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Cirque Colors Tender Touch</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ejavufup5eaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1lpmpd6</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Album Nails For a Concert 😎</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpmpd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1lpmney</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>My current favorite shade of red</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpmney</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1lplsil</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Emily de Molly "Haunted Vibes" vs MC "Nocturne"?</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lplsil</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1lplpqm</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Secret Purple Oasis</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lplpqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1lplich</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Which is best thinner?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lplich</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1lpldrn</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>still getting the hang of this lol</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpldrn</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1lpktgp</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Sheer Nude Matching!</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpktgp</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1lpjndh</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>New polish for the week!</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpjndh</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1lpjmy6</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Bi Pride Nails</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0e3arxs19daf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1lpj9z2</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Accidental Cookie Monster mani</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpj9z2</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1lpivqg</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>NPS gave a palette… how could I not!</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpivqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1lpik0s</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>LynB Fluffiest Blanket vs Glisten and Glow 3 Little Pigs?</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpik0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1lpijhp</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Showstopper at golden hour 🌸</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpijhp</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1lpfw04</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>1 Month of Growing out My Nails!!</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpfw04</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1lphecn</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>[PR] Sassy Sauce Glampire 2.0 — Hot Ghoul Summer in full effect</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lphecn</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1lph5ff</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Frosty Lime</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yhtsmsmbncaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1lph493</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Grand Canyon Mani</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lph493</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1lpg6gv</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Funny Bunny 🐰 + Moonjelly 🌙</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpg6gv</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1lpfu6t</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>June Roundup 🌈</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpfu6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1lpfhe3</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Magnetic techniques?</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7c32dml1acaf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1lpf8j3</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Perfect shimmery summer blue 🐬</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpf8j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1lpf736</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>🍋 Unacceptable! 🍋</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpf736</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1lpejf2</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Drugstore glitter grabbers?</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lpejf2/drugstore_glitter_grabbers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1lpe5e9</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>White part of nail disappearing?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpe5e9</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1lpcc53</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Welp, it was a nice 8 months 🥹</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpcc53</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1lpc73s</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Jior Couture: Celestial Goddess coming back to PPU rewind (TW long thumbnail last slides)</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpc73s</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1lpbrri</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Beach themed nail art ☀️</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpbrri</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1lpbnfz</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Dragon Nails!</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpbnfz</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1lpbc9d</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>OPI A-Rose before Dawn, Broke by Noon</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpbc9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1lpb7d3</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>I am currently doing my toes, and I’m not great at it. Quick question please!</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lpb7d3/i_am_currently_doing_my_toes_and_im_not_great_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1lpaijg</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Phoenix - Intangibility</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpaijg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1lpafhx</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Retina burning beauty</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpafhx</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1lpab4i</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Dupe for Beauty Pie Super Nude?</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpab4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1lp9yr6</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Finally had a go at a gradient 💚</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1l2as3z6baf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1lp9fu8</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Looking for a dupe of this discontinued Primark nail polish</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp9fu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1lp9fdl</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>How many coats is too many?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lp9fdl/how_many_coats_is_too_many/</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1lp9by0</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Mermaid vibes 🧜🏽‍♀️</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gpzb41m2baf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1lp976i</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Incredible color, awful formula</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp976i</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1lp9254</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>mermaid mani 🫧🐠</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp9254</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1lp8teb</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Deep sea magnetic</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp8teb</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1lp8fmx</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Six months of manicures in my journal</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp8fmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1lp83kx</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Sunset chrome on polish</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp83kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1lp7xqn</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Builder gel for nail strength?</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lp7xqn/builder_gel_for_nail_strength/</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1lp7ihk</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Having difficulty letting go of magnetics</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7c2u1m29qaaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1lp74lp</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>We Will Not Take His Shit</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp74lp</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1lp6xpn</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Eyelet Lace Nails</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp6xpn</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1lp6i53</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>I’m obsessed with Holo Taco</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp6i53</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1lp6h1p</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Do we think this is a cute combo? 💕</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp6h1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1lp6gdo</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Happy Canada Day 🇨🇦</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d65r9facjaaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1lp63j1</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Cupcake Polish Flakie formula</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lp63j1/cupcake_polish_flakie_formula/</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1lp61bx</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Blue Chrome Snow Lepord</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgtl6ro4gaaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1lp5z9i</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>I can't help but feel like this combo is giving rainbow trout.</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp5z9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1lp5t3x</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Nichibotsu</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp5t3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1lp5q3p</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>sally hansen crimson crush is a dupe for opi cajun shrimp, for anyone else on a budget this summer 🍉☀️</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zexss7eeaaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1lp2ng7</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Not really a summer colour but.. it doesn't matter. I'm obsessed</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp2ng7</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1lp4s99</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Growing out my nails again😌</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp4s99</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1lp4ktm</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Aaaaadventure Time nails</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwhe1jxr5aaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1lp3gh6</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Butterfly Wings &amp; Beyond the Sunset Leads My Way</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp3gh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1lp3fla</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>✨️🌈Glitter Gradient 🌈✨️</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp3fla</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1lp3ea0</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Square it is</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp3ea0</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1lp3dzk</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Nail tips on Brittle nails?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m64lclaay9af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1lp3br7</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Neon purple shining BRIGHT!</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp3br7</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1lp359b</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Aurora Beam vs Blowin Bubbles</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lp359b/aurora_beam_vs_blowin_bubbles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1lp2po3</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>the watermelon halves sister i didnt expect to like this much</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7wagrybat9af1</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1lp2k09</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>norpsilocin vs. butterfly wings</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lp2k09/norpsilocin_vs_butterfly_wings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1lp2iw6</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Might these nail polishes be "olive skin friendly", would appreciate feedback on them!</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lp2iw6/might_these_nail_polishes_be_olive_skin_friendly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1lp2bvt</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>this combo does somethin to me 🫦</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp2bvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1lp22ha</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Sacred Hearts ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ylndxs7jo9af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1lp20nn</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Key Lime🍋‍🟩💚</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp20nn</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1lp1zhx</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Uhm... What?!?It's too pretty I just can't even</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp1zhx</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1lp1qgh</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>What I wore in June 🍉</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp1qgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1lp1kq2</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Watermelon Nails</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp1kq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1lp1334</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Lush vs Doomicorn 2.0</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lp1334/lush_vs_doomicorn_20/</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1lp0wxw</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Multichrome and Shimmer Swatch Comparisons</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp0wxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1lp0wch</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Bf: “YoU sHoUlD hAvE dOnE rEd WhItE aNd BlUe”</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jo7z8c2cf9af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1lp0knk</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Wow, Funhouse is gorgeous!</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z3hgwkomc9af1</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1loqe6o</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Essie’s Mercury On Dupe</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdtcp3l4c6af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1loogyt</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>My first time shopping PPU so I have to share because.. stoked!</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loogyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1lozvev</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Green magic</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lozvev</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1lozsw1</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>A completely Canadian mani!</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lozsw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1loz1dn</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Second time DIY gel nail!</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5yce9zly8af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1loxw8s</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Tried stickers for the first time🥹</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loxw8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1loxq40</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1loxq40/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1lowucd</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>On Location is amazing for summer! ☀️</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lowucd</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1lpq4r4</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>greek tiles inspired nailart 🧿</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpq4r4</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1lpq3wh</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>My nails look yellow for some reason, can you help me?</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ld8t1r14faf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1lpop2z</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Jade (From Bratz) Inspired Set💋🖤</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpop2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1lpo7z6</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Thoughts on these?</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vy8mrvzvheaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1lpmtmz</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>practicing some 3d.</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dk25zaw2eaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1lp0j7w</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>new set by me🗡️🕷️</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp0j7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1lp3xgx</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>LABUBU NAILS.✨</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp3xgx</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1lpisam</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Testing the new cateye polish 😋</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ro7gcujh1daf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1lpluuy</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Today’s nails art work</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpluuy</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1lpknlt</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>First set</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/id3fmet9idaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1lpjmpy</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Game Section Gel Nail Art</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpjmpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1lpj7ou</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Don't mind how close to cuticles it got, my fingers swell</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/meisldv95daf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1lpi8x2</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Polygel sculpted nails ✨</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vajxq4sqwcaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1lpi552</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>You look like the 4th of July! Makes me want a hot dog REAL BAD.</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrtaechtvcaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1lpgxpj</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Freestyle set inspired by Lady Gaga’s ‘Telephone’ MV ✨</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpgxpj</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1lpgpi9</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Thoughts on my character art?</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpgpi9</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1lpfdak</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Did some beetlejuice nails</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpfdak</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1lpdr31</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Floral and cat eye</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mdsp9d18xbaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1lpdntv</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Here are my zombie ones from Halloween last year 🧟‍♀️</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpdntv</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1lpdd7g</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>recent press on nails i just finished! 🥹🖤</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7thchpfhubaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1lpcmtc</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Some freestyles I did this week</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpcmtc</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1lpbup7</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Rainbow polka dotted gems</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpbup7</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1lpbbqk</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Beginner Anime/Nail Art Tips</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lpbbqk/beginner_animenail_art_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1lpao51</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>I love</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mufabe8pbbaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1lpae7n</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>new claws</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xyqjbat9baf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1lpaab5</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Stars</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/an56h4j29baf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1lp9xuc</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>What can be added</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6a0bnzys6baf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1lp9rmz</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>A little compilation of the press-ons that I've made for myself in the past 3 months.💅🏼</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/czv9r0il5baf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1lp7z8z</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Eeveelution nails</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp7z8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1lp7dx9</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>I did my nails using art supplies</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp7dx9</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1lp7dq6</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Estas flores bellas son súper fácil de hacer !! Te gusta ?</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp7dq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1lp78p0</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>My stray kids nails!</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp78p0</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1lp59n7</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>As Promised, Canada Day Manicure</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp59n7</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1lp4o8f</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Jelly gel nails</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp4o8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1lp4jei</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Cute sport nail designs</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lp4jei/cute_sport_nail_designs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1lp3ufs</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>4 of July Nails</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/302sjmpm1aaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1lp3dah</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>My first attempt at gel nails at home, how did i do?🥹</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4487wh4y9af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1lp2cto</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>did these ✨️golden orchid nails✨️, 1 finger has a press on due to a small injury</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lp2cto</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1lp1uth</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Fourth of July nails done by me 🫶🏻☺️❤️and a tiny paintbrush</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21brxm5vm9af1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1lozxr4</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Fave set ever 🦋</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lozxr4</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1looff3</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Cult of the Lamb and Gloomy Bear nail sets(done by me, on myself)</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1looff3</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1loj0kl</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Our nails for our friends summer wedding!</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1loj0kl</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jul  3 08:12:53 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_06.xlsx
+++ b/data/collected_data/2025_07_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C721"/>
+  <dimension ref="A1:C926"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12690,6 +12690,3491 @@
         </is>
       </c>
     </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1lqjef6</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Jaws themed 🦈</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z60cujae2maf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1lqj6m2</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>My first official set</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqj6m2</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1lqi1jn</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Happy 4th of July!</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58hpdrlvmlaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1lqhpfd</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>I like them, but my mom says they look off 😒</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqhpfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1lqhpdj</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>fav sets so far this year</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqhpdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1lqhov7</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>if these are illegal</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqhov7</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1lqhluz</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>It only cost me $80 to turn my thumbs into toes!</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqhluz</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1lqgl3l</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>What is this on my nail??</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqgl3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1lqhafy</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>My first DIY 4th of July nails :)</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqhafy</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1lqggvo</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Pineapple Pedi</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wk25zs676laf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1lqgcxm</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Estoy muy enamorada 🥰 🩷</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpj47df55laf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1lqfjnp</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Last month's mani before the allergy</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqfjnp</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1lqfbi2</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>July 4th nails!</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rf7hsfm6vkaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1lqf9cs</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Im crashing out</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqf9cs</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1lqf3lt</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Name ideas</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lqf3lt/name_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1lqf0kv</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Palate cleanser nails</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aojnbobaskaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1lqegyc</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>4th of July nails I did for my bestie🎆</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxv5a0k8nkaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1lqdjcl</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>SO PROUD OF MYSELF</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7dbo3wsekaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1lqe9y9</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Longest my natural nails have ever been, are they healthy?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqe9y9</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1lqe46r</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>75% of the time I get my nails done, my cuticle gets cut (diff nail techs)</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lqe46r/75_of_the_time_i_get_my_nails_done_my_cuticle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1lqdtem</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Do these look grown out?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqdtem</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1lqdntg</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>New ones I did to my sister</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqdntg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1lqdmvs</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>New ones I did to my sister</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8lxlzlwofkaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1lqdke8</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>fruit salad nails 🍌</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cw9a5dd2fkaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1lqderc</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Back to acrylics since I can’t stop biting my naturals no matter what….</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9a2scqandkaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1lqde86</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Can I use polygel instead of glue on press ons?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lqde86/can_i_use_polygel_instead_of_glue_on_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1lqdckp</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Felt like a French Tips kinda week</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5wi1v33dkaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1lqdbs4</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>first time doing my own gel nails 💀</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brknr16wckaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1lqcsbn</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Nice</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5hj95518kaf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1lqcs7k</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>pressed plants glass nails</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqcs7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1lqcogc</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Y’ALL. I realized another use for my e-file. CALLOUS REMOVAL.</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4qybth27kaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1lqbnk9</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Are these nails good enough for proposal??</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71sicrpwxjaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1lqcfib</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Illuminated manuscript set I just finished!</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqcfib</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1lqcb0a</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Bad weekend to be a glizzy</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqcb0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1lqbujh</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amtrjqdozjaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1lqbffu</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>worth $85?</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etiarl42wjaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1lqb46m</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>When You Accidently Kinda Sorta, Match your Nail Polish to your Platforms</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqb46m</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1lqathf</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Hiiii first time acrylics!!!</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqathf</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1lqaa2n</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Why is it lighter in some spots? :(</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1lkv19gmjaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1lqa4v8</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>What is the best nail shape?</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lqa4v8/what_is_the_best_nail_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1lq9r1r</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Reached the longest, healthiest nails of my life. Today, disaster struck. Please pay your respects &lt;/3</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq9r1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1lq9quz</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Hi hybrid</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lq9quz/hi_hybrid/</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1lq9l25</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>If you could only have one mani for the rest of your life, what would it be?</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lq9l25/if_you_could_only_have_one_mani_for_the_rest_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1lq7x9y</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Trying to grow out natural nails and one broke.</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ksslziya4jaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1lq90fg</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>first time growing out my natural nails</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq90fg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1lq95vt</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Gel polish coming off- sweaty hands the cause?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lq95vt/gel_polish_coming_off_sweaty_hands_the_cause/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1lq8ah5</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhmhv3m37jaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1lq7zvu</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>prom nails!!!</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qncffe9v4jaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1lq7z4r</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Press On Nails</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lq7z4r/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1lq7f6j</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>How much would you pay for ?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq7f6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1lq79lg</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Cherry blossom nails for my trip to Japan!</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq79lg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1lq77t6</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Done on myself</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq77t6</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1lq74uc</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Just starting</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lq74uc/just_starting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1lq6iya</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Can I apply press on’s with a layer of polish underneath?</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b80y2bu2uiaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1lq5w48</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>simple nail art with real gemstones 💎</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq5w48</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1lq5g8j</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Need advice for diy French pedi</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gt0rtk2ojiaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1lq52h0</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>July Cat Nails!</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p02rjxuhjiaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1lq4snj</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Going bananas over my new set</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08ff1kxhhiaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1lq4849</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Just needed TWO More days!</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq4849</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1lq40k9</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Feet are weird</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq40k9</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1lq3w0w</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Sally Hansen hard as nails is breaking my nails?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/idvxzfk2biaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1lq3q2v</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Most recent set</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dympew8u9iaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1lq3bp8</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Really love this set!</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7mvhba27iaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1lq3lcu</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>I love flowers</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpr4w3xy8iaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1lq31x4</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Newest set!!</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq31x4</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1lq2wn3</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Holiday nails</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jzsrrc44iaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1lq2n2z</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Just why ?</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq2n2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1lq26jr</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>summerween 👀🩸</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/avy95993zhaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1lq1ksx</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Galaxy nails</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/662nddivuhaf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1lq1gkt</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>First time being ‘extra’</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wv0y7ac2uhaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1lq0uae</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>This sub inspired me to get back into nail art and make my first press ons</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqkj713vphaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1lq1diq</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Has anyone used either of these polishes? First is born pretty second is Gaoy…</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq1diq</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1lq0l6k</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Anyone recognize this UV lamp? Is it good?</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vb8uhmh3ohaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1lpxqc0</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Why do my fingers look like this? I moisturize &amp; use oil multiple times a day.</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9klgl1p84haf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1lpzu9e</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>🦋💎</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpzu9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1lpxkrz</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>A Modern Inspiration…</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpxkrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1lpyonu</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>July Nails 🌟</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpyonu</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1lpqqxo</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Pink and blue lily inspired set 🤭🥹💓</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jjy24d1cfaf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1lpw20k</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>matte black claws meet soft girl cheetah: rawr but make it fashion 🐆🖤</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpw20k</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1lpzpux</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>I like this shade.</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56ptg3x0ihaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1lpzpt4</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>New set done by me</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpzpt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1lpwx7c</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Made some press on nails</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/an0u1zueygaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1lpwz8b</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpwz8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1lpzg7d</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>DIY Birthday nails💅🏻</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybkx1ia7ghaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1lpxypo</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Bunny nails 🐇</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpxypo</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1lpxwkd</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>These babies in the sunlight? *Chef kiss*</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azbarq5i5haf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1lpxoyh</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Matcha manicure 🍵</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6e9adky3haf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1lpx9a3</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Can't afford nails anymore so this was my last set 🤍</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sz4em3eu0haf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1lpwrmv</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Nail glue help</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gg6k5zw8xgaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1lpwnqo</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>These bear cuties I got from Etsy 🎀 🧸 I never wear nails but I feel that my hands look so cutesy and feminine with these 🤭</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzbpk76gwgaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1lpwm2p</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Having a hard time with blooming gel techniques</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpwm2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1lpw4a9</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Keepin’ them short &amp; sparkly 🌸</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vyg4gxcsgaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1lpvzop</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Summer claws</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kga7yra6rgaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1lpve2z</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Wifey</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjvi5etmmgaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1lpvcqg</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Shiny 🤍</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpvcqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1lpvc4q</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Galaxy vibes 🌌</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ftejnoz7mgaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1lpv6tf</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>First time builder gel set!</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ns61fup2lgaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1lpv1w2</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Nails I’ve done the past couple days as a noob</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpv1w2</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1lpusmg</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>What is the proper amount of time before you get acrylics removed?</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lpusmg/what_is_the_proper_amount_of_time_before_you_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1lpujht</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>💖🧡✨</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpujht</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1lqjpj4</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>My prettiest set yet! 😍</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68jevnho3maf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1lqj6sd</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Dupe for this HHC polish?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oux1olizzlaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1lqidij</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Tried something</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqidij</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1lqic27</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Pink shimmer with strawberry milk🍓🥛</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qlmrex1qlaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1lqi5iq</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Was going for sea glass</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyo3bey1olaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1lqhv69</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Pixiestick vs Lake Superior Schenanigans</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqhv69</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1lqhk21</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Help me choose between Maelstrom, Emerald City, and Dead House</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0avx12tjhlaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1lqfx0d</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>favourite reds ?!</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqfx0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1lqfvd2</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Sour Apple Rings is back!!</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwlvf5d60laf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1lqfg0x</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>have i just found a hema free press on glue???</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lqfg0x/have_i_just_found_a_hema_free_press_on_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1lqev82</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Cirque Jelly Swatch</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqev82</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1lqenus</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Simple flower accent</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28ucyjmcokaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1lq8otf</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Thoughts on Cuticula?</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lq8otf/thoughts_on_cuticula/</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1lqaw6n</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>in search of sparkly peach color</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lqaw6n/in_search_of_sparkly_peach_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1lqdu2q</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Heirloom Manicure</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqdu2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1lqchru</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Can folks please post their swatches/manis of Dam Nail Polish “Till the Music Stops”? (Nail image is not mine)</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nopl11xe5kaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1lqca6h</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Baby poop, but make it ✨sparkle✨</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqca6h</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1lqc8pd</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>beach nails for summer 🏖️</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqc8pd</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1lqc5k6</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Got my first PPU order and I’m totally obsessed 😍💅</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/64rvtwrd2kaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1lqc4de</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>The rumors are true…</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1bwjacd22kaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1lqbqgu</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>[Rewind] Sassy Sauce – Pain in the Asteroid 2.0</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqbqgu</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1lqbhex</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>tie dye for july</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqbhex</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1lqavnk</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Happy belated Canada Day! 🇨🇦 to celebrate I’m rocking two Canadian brands for a mani my friend lovingly called “Shrek chic”</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqavnk</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1lq95td</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Inspired Sense review?</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lq95td/inspired_sense_review/</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1lq8p5d</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>One of my oldest polishes!</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq8p5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1lq8dpf</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Good news from Nailstuff.ca for Canadians!</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5geoo6bs7jaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1lq85ct</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>I’ll be like ‘I needed this’ and it’s just applying deep space 💫</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nj88dy06jaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1lq7t6c</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Fired Up!</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq7t6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1lq7qt5</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Contact dermatitis</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lq7qt5/contact_dermatitis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1lq7k2q</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>I forgot how hard it was to use regular nail polish🥵</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq7k2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1lq7e41</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>My cuticle work is messy no matter what I do</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq7e41</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1lq6y0h</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Can I avoid greenies if I apply thick layer of polish before press on nails?</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq6y0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1lq6v83</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>My best gradient yet!! Holo or no holo?</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq6v83</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1lq6th9</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Nail Art Progress</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq6th9</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1lq6h30</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>is this not cultural appropriation?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq6h30</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1lq6cct</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Not Entirely Patriotic Mani</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq6cct</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1lq6aqx</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>funeral for my middle finger</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yn8co0oesiaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1lq63ju</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>What I wore in June</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq63ju</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1lq5rtp</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Melonberry &amp; Jump Jump Bug w/ Moondust ✨🩷💜💚🩵✨</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq5qdt</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1lq5pgw</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>4th of July 💀</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq5pgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1lq5l1v</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>What do y’all do after the interview?</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lq5l1v/what_do_yall_do_after_the_interview/</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1lq5ab4</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Cuticle oil pen label got sticky??</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kcg81e3liaf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1lpicfg</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Best magnetic polish brands?</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lpicfg/best_magnetic_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1lq4ub1</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Happy 4th!</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mba6esvthiaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1lq4qp5</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Cuticle oil...it's everywhere!</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lq4qp5/cuticle_oilits_everywhere/</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1lq4m61</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Essie Midnight Ball vs. Mooncat's Queen of Chaos?</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lq4m61/essie_midnight_ball_vs_mooncats_queen_of_chaos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1lpx764</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Cracked Breakfast at Monique’s</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvgjztcf0haf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1lq3sex</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>sally hansen hard as nails is breaking my nails?</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/746p3eocaiaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1lq3eah</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>twisted terracotta tanzanite</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq3eah</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1lq2j7y</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Has anyone else been inspired by their kitty‘s colour story? 😹 My nails in the style of Shrimp instead of a 4th of July mani 😤 (he‘s worth celebrating every day of the year!!) ♡ 🐾</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq2j7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1lq2hiy</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Mixing two bottles together</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lq2hiy/mixing_two_bottles_together/</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1lq2frk</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Zoya-Maren</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq2frk</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1lq29qu</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Lurid Shop Restock</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://luridlacquer.com/collections/all</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1lq297v</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Second attempt at a French Smile with builder gel!</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z7euahd8zhaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1lq1tub</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>I was not impressed by Mooncat's To All Who Ghosted Me, until now.</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq1tub</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1lq11ki</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Inspired by something IRL</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq0kie</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1lq0esw</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Arwen and Aragorn swatches</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lq0esw/arwen_and_aragorn_swatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1lq06u2</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Emotional Support Taco</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq06u2</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1lpzz9m</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>I Dream in Green ☁️💚🩵</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpzz9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1lpz1ez</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Holo Taco price increase</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lpz1ez/holo_taco_price_increase/</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1lpyum0</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>TFW You Open a Fresh Bottle of Allergy Meds and Realize...</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sf57w3j2chaf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1lpymuc</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Enchanted polish</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lpymuc/enchanted_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1lpyagm</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Peachy glow 🤩</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpyagm</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1lpxx87</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Found a Lacquerista in the wild (pet store)!</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g3deaj5n5haf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1lpx4fi</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>ILNP - Heat Wave</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpx4fi</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1lpx49u</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>I am in LOVE!!!</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpx49u</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1lpx42y</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>From long to… so long 💔</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpx42y</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1lpwour</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>My comfort color 💜</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpwour</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1lpvyi9</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Lines on Nail</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vi693qr3rgaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1lpvyek</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Berry red in my night lighting</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpvyek</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1lpvw66</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Help me find a polish that matches my crocs!</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpvw66</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1lpv9wr</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Proud of my progress</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpv9wr</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1lpv7wp</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Londontown Mani Bright Nail Scrub</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lpv7wp/londontown_mani_bright_nail_scrub/</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1lpuwap</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Illamasqua - Baptiste</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpuwap</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1lpum3t</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Glass file recommendations</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lpum3t/glass_file_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1lpui22</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Tomatoes &amp; orange nails for summer (2nd attempt at blush nails)</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpui22</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1lpugns</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Forgot how difficult it is to paint my own nails</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/212b5x0yegaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1lpn1uc</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>another nail is growing...??</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25amph565eaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1lptoun</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Patience was needed with this one!</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lptoun</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1lptli1</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Do all glass nail files feel like scratching a chalkboard?</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0vit7vr47gaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1lptcl1</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Has anyone tried solar polish with their kbshimmer top coat?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lptcl1/has_anyone_tried_solar_polish_with_their/</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1lprmv2</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Mischief in progress 😼</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8f7hyc3jcaf1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1lqfz9z</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Beautiful Hello Kitty nails 💗🌷💅🏻</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b5xvjrph1laf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1lqf9bc</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>First time using blooming gel. Decided not to add the jelly color over the white on my other hand bc why not haha.</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqf9bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1lqe1et</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>4th of July Nails</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqe1et</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1lqci34</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Who needs red white and blue when there is purple 💜</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/puntjguh5kaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1lqcgjf</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Bunny nails</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqcgjf</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1lqaz7q</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>My first Ghibli inspired set!</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2c9al9b9sjaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1lqam4l</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Don’t look at my cuticles!!!!</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eelc0fu6pjaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1lqaeo7</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>90’s junk nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqaeo7</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1lqadyj</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Lisa Frank</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqadyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1lq8g8g</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Dots done by me ✨</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6h3ftu1b8jaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1lq80fu</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>My 4th of July set 🍒🫐🐞</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq80fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1lq7hu7</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>A Little Plaid</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq7hu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1lq6b0x</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>How are yall getting such detailed lines and doing intricate designs?</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq6b0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1lq5whm</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>This weeks nail set</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0im334qkpiaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1lq4nr2</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Made my first set!</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lq4nr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1lq1lmw</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>My friend is new to nails and loves pink. She saw mine and wanted to try a press-on set so I made her these shorties🎀</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ff1ghj11vhaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1lq1947</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Todo iba bien hasta que tocó encapsular brilloso 🫢</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oht3eiqgshaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1lpyo0o</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Color: DND 713 Orange Sherbert has been a huge hit in our virtual nail salon this summer</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8dqlh5tahaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1lpyckd</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Do you like these 🍒</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3praiy0m8haf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1lpy3ig</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>🍒🍒</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yt1z9iiv6haf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1lpx5g4</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Beachy waves vs Molten lava</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lpx5g4</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1lprl3y</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Pretty in plaid Barbie</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lprl3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1lpqqrh</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>looks like halloween came early...</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tfagbe8zbfaf1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jul  4 08:13:06 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_06.xlsx
+++ b/data/collected_data/2025_07_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C926"/>
+  <dimension ref="A1:C1140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16175,6 +16175,3644 @@
         </is>
       </c>
     </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1lrd2ss</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>My first press ones</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20c66vhhctaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1lrcte7</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Been learning to do my own nails since October 2024. This months nails is</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrcte7</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1lrcq3p</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>My summer nails</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrcq3p</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1lrcfps</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>How to shape curved nails?</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lrcfps/how_to_shape_curved_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1lrckkh</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Día de los Muertos Nails</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrckkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1lrcb7s</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Some nails I did on myself as an amateur</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrcb7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1lrbrvh</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Trying to book an appointment with my nail technician her menu is confusing need some help</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrbrvh</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1lrbnuv</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>my first time trying gel x nails :D</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrbnuv</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1lrbm3v</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Rate my new nails out of 10</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ihs1g0jfvsaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1lrbbh9</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Gel Manicure Splitting</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pj771tg6ssaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1lra5zg</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Gel X blue swirly beach nails</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lra5zg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1lra06p</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>First set. These nails are too pretty for my hands. Definitely too long.</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y8mjbyb7esaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1lr9bfv</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Did I mess up my new set?</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr9bfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1lr9xaa</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>1st time getting my nails done in years</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr9xaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1lrb08o</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>How it started , how its going 💕💅🏻</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrb08o</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1lrb1yb</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>my fourth of july nails!</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m41grd2bpsaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1lraybp</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>reverse ombré chrome french 💖</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uj7wtat7osaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1lrakaw</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>The strawberry, cherry, mushroom, and bow are stickers.</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrakaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1lr9vgk</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Forth of july nails</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr9vgk</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1lr9o1m</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Just got this set and I’m in love</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr9o1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1lr9jm6</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>i paid $180 for these 😬</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr9jm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1lr926m</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Glitter frenchyyy🥹🥹😍</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6o8chdr4saf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1lr6w8e</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Are my nails okay?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr6w8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1lr8tx0</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Cat eye</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr8tx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1lr8pkv</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Paying in full before appointments</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lr8pkv/paying_in_full_before_appointments/</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1lr8hdc</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>are these bad?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr8hdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1lr89x6</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>GelX blue swirly beach nails</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr89x6</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1lr85xc</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>I love them 😍</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uz1o5c3wraf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1lr83pd</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>I’m so obsessed with this set I just finished</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr83pd</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1lr7yxb</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>summerween 🦴</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzad0366uraf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1lr7pws</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Nail day!</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cc1jz78rrraf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1lr7n4w</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Fourth of July nails</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr7n4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1lr7c4a</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Has anyone actually purchased the ONail AI Lamp?</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kouu1fg3oraf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1lr6zeq</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>A Little 4th of July Vibe</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqpj7entkraf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1lr6w4i</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Was planning to get a cobalt blue but changed my mind last second. 💙🩵</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr6w4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1lr6sp7</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Natural nails!</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr6sp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1lr67j7</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Pokemon inspired Fluid Nail Art</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr67j7</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1lr6bdw</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Flail Nails</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hkva5gwjeraf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1lr5nvn</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>pictures on nail</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr5nvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1lr5lif</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Im in love with this color and shape</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vuxojlcu7raf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1lr5fcd</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Simple gothic nails</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr5fcd</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1lr51o3</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>At home baby blue gel nails 🩰🌊</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/375rtzqj1raf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1lr4cwd</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>I’m kinda furious 😭</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr4cwd</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1lr4cqi</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Being a nail tech&gt;</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9cqzw1twqaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1lr4bnt</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Birthday mani 💙✨♋</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr4bnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1lr3zqv</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Are nail tip sizes standardized? Do all brands use the same measurements for their numbered tips?</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr3zqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1lr3z45</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Summer nails!</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4rlo7x4ktqaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1lr3s4h</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>ALMOND SHAPED RUSSIAN GEL MANI IN RED ♥️</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcdpk0ayrqaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1lr0yh9</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Is this chunkiness normal for hard gel?</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3z3mdb3h5qaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1lr3cn5</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>almost 2 week retention!</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sxu9igqeoqaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1lr3ihc</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Dip nails replacement?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr3ihc</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1lr3i4v</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>My first time doing my own acrylics. I’m prepared to be roasted if it comes with advice :)</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr3i4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1lr36i4</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Personal nail station in progress</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzz1vnqzmqaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1lr34tu</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Happy Independence Day!</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr34tu</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1lr348h</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>First time diy-ing a fill</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr348h</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1lr32fc</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Flowers always make my day🌸</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vuq75s03mqaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1lr2yu4</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>It’s giving renaissance 🩶✨🪩</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr2yu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1lr2p76</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Which shape looks better on my hands?</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr2p76</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1lr2nb7</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>First time making fake/press-on nails</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr2nb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1lr24d1</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Told my nail tech I wanted bright pink and to surprise me!</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnxp3lqfeqaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1lr22hc</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>French💙🤍❤️😻</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr22hc</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1lr1ys2</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>how to start selling nails</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr1ys2</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1lr1ol4</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Reflective set 💎</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sdsuqy70bqaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1lr06up</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Are these nails from the salon as  “botched” as I think they are?</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr06up</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1lqz7uu</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Magnetic nails</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyrsmuxkspaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1lr0p0z</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>My Lisa Frank fantasy 🌈✨</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr0p0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1lr0e89</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>French Mani mess up?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr0e89</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1lr078h</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>rilakkuma nails 🩷</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7q2ssoiuzpaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1lr057e</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>27th birthday nails!</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr057e</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1lr044l</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>💕All the chrome pinks 💕</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr044l</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1lr02y1</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Gel-X</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr02y1</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1lqzzno</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>They look prettier at night</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dodbt3m9ypaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1lqznzl</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Got the video to work here is the sparkle ✨ in action</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d4srobyqvpaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1lqzn4i</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Etsy press-on recs?</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lqzn4i/etsy_presson_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1lqz91l</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>My comfort zone with the nails is to add a slight layer of glitter on a nice color</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqz91l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1lqysc1</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>BDAY NAILS!!!</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwrkyw0gppaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1lqyrsw</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>nail day 🐆🍒 (credit to Jocelyn @ Get Nailed as always)</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edrg3x2cppaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1lqxqpb</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Toe Thumbs</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqxqpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1lqy62h</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Bump on nails?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqy62h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1lqxl16</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Still love this kind of nails at 27</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgyrf0frgpaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1lqxdt6</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Serving Bikini Bottom</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dsrwyrwbfpaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1lqx953</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>I’ve been practicing and I’m proud of this set 😊</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqx953</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1lqx3ps</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Three months as a nail tech</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/233ho5scdpaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1lqwnia</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Any Luminary sales coming up on their website?</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lqwnia/any_luminary_sales_coming_up_on_their_website/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1lqx0i9</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>4th of July nails!</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykr2wcvpcpaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1lqwwxg</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Just plain white 😊</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jr4a2f90cpaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1lqwvk3</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Star Wars set✨</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ztd52yobpaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1lqve88</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Best lamp for drying nails (non-gel) at home?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lqve88/best_lamp_for_drying_nails_nongel_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1lquzgy</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>How do you use these Nail Drying Drops?</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhforwigyoaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1lquywy</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>at home nail tech and cats</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lquywy/at_home_nail_tech_and_cats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1lqup72</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>These may not be everyone’s cup of tea but I’m proud of them!!</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqup72</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1lquo7q</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Beachy</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1g311jmbwoaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1lqql85</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Post builder gel removal</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqql85</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1lqs9em</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>What should I ask for or what colors should I choose for nails like these at a standard salon?</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lqs9em/what_should_i_ask_for_or_what_colors_should_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1lqsn3x</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Nail Inspo</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7z2h69uhoaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1lquhvl</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Advice from nail techs on how to start?</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lquhvl/advice_from_nail_techs_on_how_to_start/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1lqu2yn</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>My newest set 🤍 I wouldn’t normally do coffin shape or white nails so something different!</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqu2yn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1lqtt5u</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>My new summer nails! I drew my vision, and my nail artist brought it to life perfectly</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqtt5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1lqtmd0</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Take Two</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/842pvazsooaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1lqtehf</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>minimalistic and perfect🤍</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93tij8c7noaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1lrd92i</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>China Glaze Sin-Derella</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ptswo0ietaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1lrbzqu</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Will somebody who owns this Essie nail polish try it over brown like this TikTok comment suggests, so I can have my curiosity satiated?</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdw7r1vpzsaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1lr93fp</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>First time making press ons</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wd3r68y35saf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1lr91fp</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Crystal Knockout Realignment</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr91fp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1lr84pa</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Acetone Antidote Scents</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lr84pa/acetone_antidote_scents/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1lr7rxg</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Non-gel magnetic polishes?</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lr7rxg/nongel_magnetic_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1lr7erz</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Help Finding a Top Coat</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/707o2xlsoraf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1lr6v3e</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>A Galaxy Far Away</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8sna5cojraf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1lr6mpv</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>summer peach jelly/crelly?</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecyu0a2ihraf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1lr6kq1</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Finally mastered the glass bead magnetic effect</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p8mv0ygygraf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1lr6ibr</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Funky Fingers (I miss this brand! 😭)</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i267nrndgraf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1lr66yk</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Pokemon inspired Fluid Nail Art</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr66yk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1lr64w4</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Holy cow 🤩</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h57ddf5xcraf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1lr62f6</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>So sad about this! I don't even know what I broke the nail on.</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://imgur.com/gallery/J3ZU1Mh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1lr5khn</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Update to my previous post</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y83s5xto7raf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1lr54oz</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>It glows!</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr54oz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1lr52jd</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Essie Purple Color - Help Finding Shade</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iq2je6w43raf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1lr51se</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Experimenting with magnets</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2qqp7amx2raf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1lr4sfv</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>I'm sorry Lady Liberty 🗽</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr4sfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1lr4hw9</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Stumbled upon indie polish in Detroit!</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr4hw9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1lr4g7p</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>June Manis</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr4g7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1lr401r</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>a mermaid has no tears ✨</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr401r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1lr3tr7</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Let it Glow</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr3tr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1lr3rp8</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>4th of July Nails 🩵 💙</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8fkpj5rtrqaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1lr3pgn</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Dupe for Neptune’s Sand?</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d48bfalbrqaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1lr3f2s</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>It was my lucky day today! I scored all of these for 97 cents each at a thrift store</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr3f2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1lr37f7</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Birthday mani 💙✨♋</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr37f7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1lr325q</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>I gave up and am doing something different</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0i9zhls0mqaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1lr2sxv</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Zoya 4th of July Sale</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhg0wghxjqaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1lr260v</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Does kerasal damage nail polish?</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lr260v/does_kerasal_damage_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1lr1z07</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Heart of Iceland</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3614mnt9dqaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1lr1u2x</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Ugliest polish 🤝 prettiest polish</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr1u2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1lr1nln</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Flakey festival nails 💃 It’s giving stained glass window 🪟</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr1nln</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1lr1l0d</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>My nails are too damaged to paint so I convinced my boyfriend to let me paint his to scratch the itch</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr1l0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1lr1cmo</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Multiple Coats with magnet?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lr1cmo/multiple_coats_with_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1lr0vdq</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Are my polishes getting heat damage?</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lr0vdq/are_my_polishes_getting_heat_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1lr0tco</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>🖤🤍</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr0tco</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1lqymf3</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Glitter Grabber Needed?</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.kbshimmer.com/what-a-peach-nail-polish-ppu-april-2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1lr0f1b</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>4th of July Nails</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr0f1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1lr0onv</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Back again</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr0onv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1lr0hsy</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Any suggestions/swatches for BRIGHT ORANGE shimmer jellies?? Thank youuuu</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lr0hsy/any_suggestionsswatches_for_bright_orange_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1lr0hn5</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>American Dream? Nah, American Nightmare🧨</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr0hn5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1lr0dd5</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Wowsers 😍</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i3vcvsl31qaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1lr0abe</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>4th of July No Stars</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr0abe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1lqzw6i</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>💙 Painted Polish Oh My Stars ❤️ and 🤍 Party Like A Patriot 2.0 🇺🇲</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqzw6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1lqzu94</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Drowning my demons in this color 🥰💚💙</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqzu94</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1lqzbea</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Looking for the best hot pink and/or fuchsia polishes...</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lqzbea/looking_for_the_best_hot_pink_andor_fuchsia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1lqyr6x</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Direct Sun</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7kb3wq97ppaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1lqylvo</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Finished my first velvet effect mani.. and managed to chip it already :')</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqylvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1lqygei</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Somethin new</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqygei</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1lqy8cb</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Persephone 🥀</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqy8cb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1lqxsaq</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Alternative 4th of July Nails 2.0</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqxsaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1lqxply</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Getting better all the time</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqxply</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1lqxoo1</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>They are FAR from perfect, but they make me really happy</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqxoo1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1lqwzp5</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>✨️🌈Rainbow Grid🌈✨️</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqwzp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1lqwf3d</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Orange Sherbet Color 🤨</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqwf3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1lqw922</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Love this shade, iffy on Mooncat though</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqw922</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1lqw881</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Reverse nail stamping is hard!</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqw881</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1lqvt0n</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>🍏🍉pink and green</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqvt0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1lqvqk7</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>I need to brag on Cracked for a moment...</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqvqk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1lqvnqp</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Sparkles even in low lighting</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gdcgtxn53paf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1lqumbu</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Comparison between PFD's Quite Literally Dead Inside vs Ether Dragon?</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lqumbu/comparison_between_pfds_quite_literally_dead/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1lqulv2</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Here's my 4th of July mani--burning embers</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yq1qzguvoaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1lqufhx</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>This one goes to 11…11:30</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjeoeehluoaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1lquf7l</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>What's your WORST photographing polish?</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7pn8pkjuoaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1lqu9gn</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Pastel unicorn gradient</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqu9gn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1lqts5k</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>What’s your favorite silver magnetic polish?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lqts5k/whats_your_favorite_silver_magnetic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1lqtr51</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Anyone know about Glam Polish's beliefs?</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lqtr51/anyone_know_about_glam_polishs_beliefs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1lqtldx</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Blue green double magnetic</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ijzgtmyhooaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1lqtf1d</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Lisa Frank but make glowy and subtle</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqtf1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1lqt5bs</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Fireworks!!</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqt5bs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1lqsa2a</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Holy bliss 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/81b5bz53foaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1lqs23i</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>ISO: Thunderstorm Blue polish</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lqs23i/iso_thunderstorm_blue_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1lqrnnp</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>First time ordering from Painted Polish and I'm in love</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqrnnp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1lqrev0</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Larger indie brand marked my order "shipped" within turnaround time, but hasn't dropped it off at the post office for a week now</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lqrev0/larger_indie_brand_marked_my_order_shipped_within/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1lqrcib</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Going through a really hard time lately, impulse bought a load of polish</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqrcib</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1lqqybe</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Neon gradient cause it’s HOT outside</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/HnxQQmd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1lqqni2</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Lemons!</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqqni2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1lqqf69</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>DIY Organization Idea</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqqf69</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1lqq9gc</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>I think I like flakies</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqq9gc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1lqpnls</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>ILNP - Hypnosis</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/th48vz0qvnaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1lqpjgw</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Essence 79 grape escape</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqpjgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1lqpatq</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>July 4 protest mani</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ru4g70fwsnaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1lqp2wr</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Flower nails to match my daisies</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99m9plo4rnaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1lqors7</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Cool on warm clash</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqors7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1lqo3ak</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>It's giving Unsweet &amp; Extra Bold✨️</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqo3ak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1lqn0ja</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>What a faff</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cmd4r0ba8naf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1lqmkuc</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Tempted with envy 👑🔮💜</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqmkuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1lqlo6f</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Give it Back Tenfold</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqlo6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1lrcqyp</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>New summer set</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrcqyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1lrcjog</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Dia de los Muertos Nails</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrcjog</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1lrbuom</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>FISH NAILS!!!</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrbuom</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1lrbtud</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Did these for my beach trip a while back</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tmb0y9ctxsaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1lrbcmh</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>First time</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrbcmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1lrafkt</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Some nail art I've done this week</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrafkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1lr8s2u</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Round 2?</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr8s2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1lr8qo2</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Some basic rocket pop 4th of july nails</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrpyewin1saf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1lr8eg4</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Hand-painted One Piece nails — I really tried 💅</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr8eg4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1lr6uyt</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Hand painted liquid chrome</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/shw69y4njraf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1lr4tpu</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>this is as patriotic as I can get</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q74mq2wx0raf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1lr4rtj</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>4th of July nails 💅🏼 🎆</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nsmu5hh0raf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1lr458r</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Super proud of this set💖</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr458r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1lr3sd7</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Este color y diseño 🥰</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9k761nwrqaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1lr39yt</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>My Independence Day creations.</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85byvx7snqaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1lr38xl</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>some nails i’ve done!</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr38xl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1lr2zbh</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr2zbh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1lqz86t</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Any idea on how to do this</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2h0q28nspaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1lqygln</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>French tips by me over chrome powder ✨</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t7ozc0u1npaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1lqtp8f</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>My first DIY nails for Independence day!</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqtp8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1lqt6aa</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Fishing lure trend</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xz6kja1lloaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1lqsho9</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Nail art I've done over the last year</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqsho9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1lqs6j3</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Inspired by a nail artist on IG.</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqs6j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1lqrv94</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>I finally figured out chrome isolation!</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emqykvpccoaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1lqrl7d</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Hard gel with cat eye and dried flowers 🌺</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v9bwwfqdaoaf1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jul  5 08:11:22 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_06.xlsx
+++ b/data/collected_data/2025_07_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1140"/>
+  <dimension ref="A1:C1351"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19813,6 +19813,3593 @@
         </is>
       </c>
     </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1ls4nxb</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Self Made Nude n Brown Gradient</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlyx4ov6i0bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1ls4kcl</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>I'm trying new techniques</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afbooc6zg0bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1ls4bfw</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>My last 3</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls4bfw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1ls4add</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>do i go refund or new salon?</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rhhli7ugd0bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1ls452h</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>First time doing press on.</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls452h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1ls3q8k</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Would gel nails look off after 10 days?</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ls3q8k/would_gel_nails_look_off_after_10_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1ls3ikj</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Vacation nails. 🦋🪼🐋</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls3ikj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1ls31jd</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Glitter glizzys</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls31jd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1ls3dxe</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Anyone else feel like they’re playing Tetris?</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls3dxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1ls2jhb</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls2jhb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1ls2end</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Nails I got done yesterday!!!</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls2end</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1ls198p</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Americana</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls198p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1ls0fgh</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>I need some help with tiny sharp top coat spikes, I'm guessing bubbles?</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls0fgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1ls11ux</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Happy 4th of July! 🎆</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls11ux</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1ls0y7r</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>I love 💕 💗</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls0y7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1ls0m84</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Finished painting the Hercules nail set! Will definitely paint more characters I just love them all!</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ssqhaexk7zaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1ls0hel</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>first time i got stilettos. i've also never had nails that are an inch and a half long</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls0hel</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1ls0392</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>First french mani</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls0392</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1lrzqsu</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Tried semi-cured gel nails for last minute July 4th party and I'm in love</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrzqsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1lrz9k1</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>birthday nails 🤍🌸</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrz9k1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1lryu2t</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Tried Something New: French Tip with Delicate Flower Design</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lryu2t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1lryemj</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Are they healthy, how can I improve looks ?</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lryemj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1lry1td</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>My daughter (34) and my (68) new look. Pedi Day Next!</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mkxr77d3gyaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1lrxv4d</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>My manicure speaks louder than words</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tdivy5k1eyaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1lrxp61</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>I need your honest opinion/ advice</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrxp61</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1lrxo3k</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Long nails for today's class</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7sp3y0p5cyaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1lrwu27</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Do any of you use jojoba oil for your cuticles? Do you think it compensates a little for using gel?</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lrwu27/do_any_of_you_use_jojoba_oil_for_your_cuticles_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1lrx042</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Pretty proud of these!</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrx042</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1lrwhv4</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>I love these nails!</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrwhv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1lrw2xs</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>This is the first time in my life I’m not wearing nail extensions. This is a Russian manicure + BIAB gel overlay. (Cuticle close up in the second photo)</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrw2xs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1lrw27u</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Happy Fourth!!</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrw27u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1lrvsxw</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Quickest way to apply gel?</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lrvsxw/quickest_way_to_apply_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1lrv4fx</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>What kind of nails are going to be less harmful to my actual nails?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lrv4fx/what_kind_of_nails_are_going_to_be_less_harmful/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1lruc4w</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>First time doing freehand nail art</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pyz02muhxaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1lrtwhv</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>So I purchased Beetles nail builder gel from Amazon and looking for alternatives</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxadxpd6exaf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1lrv9yo</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Is this normal</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrv9yo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1lrv54x</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Is it as bad as I think?</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrv54x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1lrv190</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Are these too thick?</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrv190</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1lruzea</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Something feels off…</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lruzea</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1lrujop</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Had to chop the nails for my new job, but hopefully they are pretty little stumps</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvlqp23njxaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1lruf11</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Where is this tint coming from?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lruf11</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1lruarw</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Is it normal for my nails to still be hurting weeks later?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lruarw/is_it_normal_for_my_nails_to_still_be_hurting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1lru30w</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Summer Marble nails</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lru30w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1lru0uo</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Clionadh - Psilocin</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lru0uo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1lrtvy8</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Dumb question about gel nails</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lrtvy8/dumb_question_about_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1lrtk2i</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Claws</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlju9e4abxaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1lrssr0</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>got these done today</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tmi613415xaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1lrsdry</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Sabrina Carpenter nails 💋</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oi4nsn7m1xaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1lrsbmz</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>4th of July Nails</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8nzbixx41xaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1lrs2ig</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Noticed this after removing gel polish. Is it a ring of fire? What are the small tiny black lines on my nails?</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrs2ig</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1lrrsug</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Happy 4th!</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrrsug</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1lrrma0</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Stabby and glittery</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8mdxegdivwaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1lrr55i</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>What’s the proper term to getting gel nails without the tips?</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lrr55i/whats_the_proper_term_to_getting_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1lrr4y1</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>I just got my nails done for the first time in 30 years and I have questions.</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6sfzr8porwaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1lrretf</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Nail tech crushed it again!</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3h2k7ogutwaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1lrqz0t</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>First time using press on nails</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xojkzepdqwaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1lrqs78</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3pgdhb3towaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1lron2k</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Switching to classic manis for good</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lron2k/switching_to_classic_manis_for_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1lrqn68</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Happy 4th (;</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrqn68</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1lrc5u8</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Confusion regarding nail care</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxy54vmn1taf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1lrgzpd</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Nails damaged after using cuticule pusher</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lrgzpd/nails_damaged_after_using_cuticule_pusher/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1lri5t0</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Rate my nails</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lri5t0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1lrj6cu</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Elden ring inspired what I asked for and what I got</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrj6cu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1lrqb2c</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Magnetic gel + isolated chrome = *chef’s kiss* 👌✨</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrqb2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1lrpyug</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Fresh set 💅</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oi1rf7gniwaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1lrq1ie</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Happy 4th y’all!</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2en9fi87jwaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1lrpx4g</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Builder gel started coming off after a week, what can I do?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lrpx4g/builder_gel_started_coming_off_after_a_week_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1lrpsmy</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Nails for my friend!</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kew6ruubhwaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1lrpr8n</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>My press ons aren't staying on</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lrpr8n/my_press_ons_arent_staying_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1lriop3</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Why is my nail so asymmetrical? Please help</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r679js7ozuaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1lrk6wc</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Nail solutions for really short and damaged nails</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lrk6wc/nail_solutions_for_really_short_and_damaged_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1lrplhw</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>can i tell my nail tech to not use e file near cuticles</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lrplhw/can_i_tell_my_nail_tech_to_not_use_e_file_near/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1lrlflo</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>My first time going to an independent tech, she did amazingg!!!</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrlflo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1lrpld4</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Reconnecting with my catholic upbringing</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrpld4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1lrn5t8</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Weak, thin, bendy nails and working with my hands. What can I do to add length and strength?!</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lrn5t8/weak_thin_bendy_nails_and_working_with_my_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1lrdf11</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>New to Nail Care, What do these mean??</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lrdf11/new_to_nail_care_what_do_these_mean/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1lrpjtf</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>new set by me</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrpjtf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1lrpbo9</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>DIY - Gelx Fill with Cat Eye tips</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smnzabksdwaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1lroz4u</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>How are they?</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lroz4u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1lrow19</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>I think I should have put another color in the 3D</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgnb7z0oawaf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1lroco2</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>How’s this??</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lroco2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1lrnch0</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Is it okay to ask for them to re do these? They are way too thick for my liking.</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cz9srth7zvaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1lrn00m</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Americans Are You still Paying for Nails? 💅🏽</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lrn00m/americans_are_you_still_paying_for_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1lrmzws</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Just got them done 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/184s06nlwvaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1lrmz6m</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Not sure what to think about this French set..</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrmz6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1lrmsmg</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrmsmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1lrmn15</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Sunset Nails</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tph0hcxttvaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1lrlvw2</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>first time trying gelX :D</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrlvw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1lrl1ov</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>4th of July nails are kitty approved!</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oz1vxb93ivaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1lrl10s</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>My Birthday Set</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrl10s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1lrksxb</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>My fully natural nails!</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrksxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1lrksdw</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Space nails</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrksdw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1lrkl3j</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Purple patchwork 8647</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrkl3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1lrk675</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Soft gel extensions</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zf6kx4jjbvaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1lrjq5y</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Jade Cat Eye With Gold Accents, by me</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tsta9k848vaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1lrjhs3</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>I love this set 😍💖</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tt9x28396vaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1lrjb5x</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>My first attempt at French mani. How'd i do?</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrjb5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1lrj9wa</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>First time builder gel set - updated!</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sbfynb0i4vaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1lrj5vk</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>vacation set</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrj5vk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1lrj5ew</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Shark week nails 💅</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99ksxakh3vaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1ls2wjx</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Why do some sellers charge tax?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ls2wjx/why_do_some_sellers_charge_tax/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1ls2big</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Se cute little strawberry picnic nails!</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls2big</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1ls28f5</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>These Nails are really pretty!</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xiu2hgtdpzaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1ls1c9x</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>My country means more to me than the crimes of the current regime</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls1c9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1ls0w5y</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Monsoon season mani🌧</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r73r46flazaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1ls0vn4</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Any Polishes Similar to Ethereal Lacquer's Under the Sea?</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khmsnj1gazaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1ls0ma2</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>People who repair computers, what do you do about your nails?</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ls0ma2/people_who_repair_computers_what_do_you_do_about/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1ls0l6c</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Wearing “F*ck” by Bees Knees Lacquer for this “Independence Day”</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjzsuwp97zaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1lrzxsr</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Muted Fourth</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ebceywt40zaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1lrzve3</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Friday night swatches!</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrzve3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1lrzpb7</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Peel Off Base Coat  not needed (day 3 mani)</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pt7r9hkoxyaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1lrzeg7</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Iconic Amber</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrzeg7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1lrz4wf</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Blurple Skittle 💙💜</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrz4wf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1lryv7t</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Sponged Stripes 🚀</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2apnq3proyaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1lrya9j</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Shifty green goodness</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lm8kncdliyaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1lry1ac</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Show your 4th of July nails</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/btovzkuxfyaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1lrxob5</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>It's *not* that girl..</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bh7oich5cyaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1lrxg5o</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Holy nail beauties 🤩</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lrxg5o/holy_nail_beauties/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1lrxem3</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>How did you spend your Thursday night?</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrxem3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1lrx322</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Wavering independence</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrx322</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1lrv119</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>❤️🤍💙</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrv119</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1lrvlz4</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Holiday split mani</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrvlz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1lrvjxp</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Gel x Tips for the Win!</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pjg4q74esxaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1lrvdcz</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Hot Damn Anthurium</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6e3hlv5rqxaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1lruxoh</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Seche Vite changed my life</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lruxoh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1lruqhm</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Whispers of Camargue</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lruqhm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1lruq32</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>My favourite colour on me: ILNP Dakota!</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lruq32</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1lru14e</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Clionadh - Psilocin</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lru14e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1lru0tf</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>My attempt at velvet nails as a novice!</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ir34dgezdxaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1lrtrs9</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Playing with color combos</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrtrs9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1lrtp5k</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Festive AF</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrtp5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1lrtkfl</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>blue opal polish of my dreams</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrtkfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1lrt4s3</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Not here to celebrate the US, but I like fireworks</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrt4s3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1lrsdlo</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Looking for inspiration! Auf der Suche nach Inspiration.</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lrsdlo/looking_for_inspiration_auf_der_suche_nach/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1lrs32g</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Solar thermal nail polish!</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrs32g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1lrrzx8</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>This is what I consider fun on a Friday night</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrrzx8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1lrrzmi</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>First time trying Emily de Molly!</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/te3i2o2fywaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1lrrtem</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Nobody here needs to know this but Bees Knees Lacquer is having a Spring Cleaning sale right now</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lrrtem/nobody_here_needs_to_know_this_but_bees_knees/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1lrrphe</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Polished for days must haves?</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lrrphe/polished_for_days_must_haves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1lrrn2p</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Baroness X Scents</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lrrn2p/baroness_x_scents/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1lrqyrd</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Issues with Nail Stamping, Polish separation on Stamp</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aejgfxv9qwaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1lrqscy</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>My take on a 4th of July mani</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrqscy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1lrqqhb</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>First try of magnetic nail polish. I’m mesmerized.</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5h4g4ziowaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1lrqfer</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Kur illuminating nail concealer</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzpz33a7mwaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1lrqeaz</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Help me find this polish</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrqeaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1lrq7pe</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Not as creative!</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0so8qfuikwaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1lrq4t2</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Fireworks! (But make it rainbow)</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrq4t2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1lrppfr</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>I Cairn Dig It! So do I need Oil on Canvas too? (PPU Folks)</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrppfr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1lrpn0a</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>New to Me Brands</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrpn0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1lrphqv</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Not feeling patriotic, but I have polish to try</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12dl1au1fwaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1lrp8l1</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>We represent this flag, not a single temporary person</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xalz1t6dwaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1lrp3we</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>This Years 4th of July Manicure</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20xemujacwaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1lrotir</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Help! Looking for Long Lasting Polish</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lrotir/help_looking_for_long_lasting_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1lromlg</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>July Jewel Beetle 🪲</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lap2yvnp8waf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1lrol6l</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Happy fourth yall</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zgwt5twe8waf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1lrokif</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>F*ck this Sh*it</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrokif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1lrnkeg</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Inspired Sense - Where's My Chauffeur</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jk1pq0u50waf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1lrnf9a</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Magnet life problems - for us non-professionals, how do you store your magnets?</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xd8o3cdszvaf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1lrnbuh</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Ruby red for July's birthstone!</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/svbibjv2zvaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1lrmyik</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Celebrating the good things today like pink sparkles</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrmyik</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1lrmqxf</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>More proud of my manicure than my country…</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dmu7x0muvaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1lrmkx0</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Difference between nail polish thinners?</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lrmkx0/difference_between_nail_polish_thinners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1lqtsan</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Jen &amp; Berries - Haul Review w/ July ‘25 PPU Rewind ‘Valley Girl’ &amp; July ‘25 HHC Overstock ‘Hollywood Handshake’</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lqtsan</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1lquq4w</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>HELP! Don’t shoot the messenger</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kenfyknwoaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1lrm7ey</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Question: Miracel Gel top coat, or other QDTC?</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lrm7ey/question_miracel_gel_top_coat_or_other_qdtc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1lrlu64</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Obsessed and dupe/similar needed</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/le5qnbk6nvaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1lrloib</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Wavy Ocean Nails 🌊⛵️</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrloib</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1lrlcay</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Dissent is patriotic</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amf2rse8kvaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1lrl947</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Mourning the death of democracy today.</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ez6q7kljvaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1lrl80s</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Cracked “blood orange sangria”</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrl80s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1lrkvqq</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Matching nails with my son for 4th of July</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrkvqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1lrktaf</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Maybelline Fast Gel - #300 "Blissful Blue" (discontinued)</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrktaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1lrkpfq</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Barbenheimer Duo available now at Apocalypse Polish</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z409ciwcfvaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1lrkp4c</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>First time doing a sponge gradient. Tips/tricks appreciated!</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkobfz4jfvaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1lrkm12</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Patriotic Nails</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrkm12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1lrjzld</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>love a pink with a blue shimmer</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r40ke9m5avaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1lrjmgs</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>4th of July</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gx7bf2b7vaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1lriqrw</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ozr0kan50vaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1lriogu</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>ILNP Rosewater</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5ap1qjmzuaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1lriim6</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>How important actually is it to use a base coat?</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lriim6/how_important_actually_is_it_to_use_a_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1lri1g2</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Petals + Melody make the perfect summer gradient</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmmiqrm4uuaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1lrhu0s</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Take me to the beach, please!</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrhu0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1lrhnr6</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Polish has allowed me to find the joy in little things this week.  Here’s The Fields and Forests of My Youth ❤️</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrhnr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1lrhja5</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>4th of July adjacent nails ✨🎆</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pedge68lpuaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1lrhgnj</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Do I need Glampire if I have Cock a Doodle Doom?</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrhgnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1lrh5wm</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>trying to book an appointment with my nail technician her menu is confusing need some help</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrh5wm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1lre61w</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>None of us are free until all of us are free. 🔥</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lre61w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1ls499l</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Guess how long this took? 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbriv4r3d0bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1ls40dq</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xf75jov5a0bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1ls3kx9</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>My bf said I nailed it (literally). Updated the crew — how’s Nami now?</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls3kx9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1ls0gf4</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Happy 4th of July 🎆</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yb13qipc5zaf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1ls0ll1</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Finished painting the Hercules nail set! Will definitely paint more characters I just love them all!</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g09mwd9e7zaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1ls04z0</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Hearts of chrome by me ✨</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrday9hb2zaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1lryrag</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Classic French Tip... with a Floral Twist 🌸💅</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lryrag</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1lryjzp</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>🌸🤍🌺</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hyfk7f7glyaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1lry7p5</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Fourth of July Nails</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06d3bz1whyaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1lrx0ii</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Pretty proud of these!</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrx0ii</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1lrvn4t</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Un poco de color por aquí!</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrvn4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1lruhhg</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Witchy Vibes for July</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gikjkkw3jxaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1lrr6u4</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Set I did today 💚🧸</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ex32q663swaf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1lrqd7q</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Happy 4th of July</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrqd7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1lrn5bv</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Press on beginner</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrn5bv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1lrm61q</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>At home Cinderella inspired (?) nails 🫧💙</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lrm61q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1lrlh5u</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Can people post their cute short square nail designs? So hard to get inspo when everyone has beautiful long nails🥲</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lrlh5u/can_people_post_their_cute_short_square_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1lrgzei</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Art nail ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ellmxc6hkuaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1lreo8q</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Why are there bubbles in my nail polish</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13oipfojvtaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1lr9ac6</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Shine bright like a diamond 💅</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00yitl417saf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1lr602u</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Pretty nails</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zo68hkvpbraf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1lr43al</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>So I really wanted to share how my press-ons look like after two weeks 🥹</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lr43al</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1lqh6s8</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Moolisa from Bob’s Burgers.</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikqmovlodlaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1lqfqn7</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Ready for July 4th 🎆</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yaak6r38zkaf1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jul  6 08:10:54 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_06.xlsx
+++ b/data/collected_data/2025_07_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1351"/>
+  <dimension ref="A1:C1540"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23400,6 +23400,3219 @@
         </is>
       </c>
     </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1lsvvmz</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>3D samples</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/htxj4uwhn7bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1lsu52u</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>How to prevent uplifting?</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lsu52u/how_to_prevent_uplifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1lstx8o</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Can you guys believe these are press ons!</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8uvq9psf07bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1lstsev</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>look at these babies grow! ☺️🙏🏻</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgqzc1iyy6bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1lsth69</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>What do we think of my nail tech?</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsth69</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1lst2a0</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Orange so real, I almost licked my nail by mistake😅</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jnflypvq6bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1lssvso</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>She didn’t just say yes… she wore the whole story on her nails 💍.</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4bz7pmvo6bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1lssu7c</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Absolutely obsessed</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lssu7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1lssg3b</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Snake Blossom  Set🐍🌸</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lssg3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1lsrygi</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Nail art ideas.. I need more</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5o4euve7f6bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1lsrpft</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Added some flowers to this set</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsrpft</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1lsrayw</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Pretty Pearly Gel set</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jpcrx4g86bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1lsqhqy</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Bendy Nails: Not Even a Saga</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lsqhqy/bendy_nails_not_even_a_saga/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1lsqctj</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Scared to get acrylics done again because of bad service</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsqctj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1lspzq3</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>July nails</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lspzq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1lsqz53</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>New set with matching black pedi 🖤🖤</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsqz53</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1lsqy95</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time (30F)</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x3asub7t46bf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1lsqeja</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>New set ❤️</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r05hp1j7z5bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1lspxt4</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Dollar Tree came in clutch for last second 4th of July press ons</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/meqig43mu5bf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1lspggq</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>my most perfect manicure !</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eu1bcrasp5bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1lspcyl</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>4 months growing out my rings of fire 🔥</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkyhzq1yo5bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1lsp9a7</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Velvet nails are really something else</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsp9a7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1lsnvwa</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>B&amp;W French Stiletto</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsnvwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1lsop5l</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>i want to get no manicure nails, what are your past experiences?</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lsop5l/i_want_to_get_no_manicure_nails_what_are_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1lsoj49</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>can superglued charms be removed</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lsoj49/can_superglued_charms_be_removed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1lsnunn</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Sunset gradient 😻</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ob23eycra5bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1lsnhe2</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Nana Nails</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsnhe2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1lsnddi</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Are these hand made press on nails sellable?</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsnddi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1lsnb7e</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>what i asked for vs what I got</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsnb7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1lsn87a</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Is lumpiness expected/normal for gel manicures?</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsn87a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1lsn7s5</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>new to acrylics… looking for advice</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9sx10f055bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1lsmnam</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Is this worth $35?</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsmnam</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1lsmjou</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Is it normal for shops to reuse acetone?</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lsmjou/is_it_normal_for_shops_to_reuse_acetone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1lslvbj</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Ombre 😍</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lslvbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1lslp5n</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Pastel Tropical Vibes🐠🌺🥥</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqg3dvzhr4bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1lsl8ju</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Beachy nails for summer 🏝️</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsl8ju</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1lsjs5t</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>How to avoid this adhesive tab line with press ons?</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsjs5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1lskrqi</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Nails I did last month but forgot to take a picture until After I took them off</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/png43v73k4bf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1lskr1j</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Summer Nails!</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxhxj28xj4bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1lskf5a</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Yay or Nay?</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0vl8wks7h4bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1lskcsy</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Gel nail polish on natural nails</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lskcsy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1lsk42g</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Are these kind of nail polish removers bad for nails?</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ahbuncjre4bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1lsjnz0</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Coffin nails. Usually I do an almond shape.</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7fm0y38b4bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1lsjkf2</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Girls day nails in Colombia❤️</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rh9asr9ea4bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1lsjgkz</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Tim burton nails 🥹🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cbtmpx5k94bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1lsjazv</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>First time posting</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsjazv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1lsix2v</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Another new set</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gb0f0ob754bf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1lsiqhl</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>any advice?</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lsiqhl/any_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1ls50ni</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>What are the different bits used for?</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jkq90ummm0bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1lscswq</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Did the Nail Tech do a god job?</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lscswq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1lrz77a</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Am I being a Karen on this tech?</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lrz77a/am_i_being_a_karen_on_this_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1ls50tg</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Gel allergies...</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ls50tg/gel_allergies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1lsezsb</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Went with Resident Evil inspired</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsezsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1lsi3b6</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>In love!</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1httxh4ky3bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1ls62m3</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>How it started, how it’s going 🤞🏻</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls62m3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1ls7k0l</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Outcome vs inspo</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls7k0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1ls8d9x</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Bite free</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ol94cmpkq1bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1ls9usk</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Gap between natural nails and gel extensions???</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zvlse7xn42bf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1lsfcxg</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Hiii these are my nails</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsfcxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1lsh9p9</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Nails done by my friend who's a beginner</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsh9p9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1lshruq</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>I aimed for opulence, may have achieved gaudy instead</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lshruq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1lsh3e1</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Growth over 8 days</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsh3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1lsh1vi</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>First time doing gel nails after a few years! How did I do?</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ni04atocq3bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1lsgz9p</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>💋🍒</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsgz9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1lsgedk</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>New nails for the month! :)</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70e3g0lal3bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1lsg3yd</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>In honor of the fluffiest Sanrio legend… Pompompurin supremacy!</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsg3yd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1lsfsx2</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Do you find it pretty?</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsfsx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1lsfs0o</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>best way to strengthen thin peeling nails?</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lsfs0o/best_way_to_strengthen_thin_peeling_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1lsf8ud</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>just finished this set!! love the lil tooth :,)</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsf8ud</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1lsf7rb</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Rings of fire care</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsf7rb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1lsf5qw</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>spring/ summer nails</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsf5qw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1lsf53j</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>What are your thoughts on nail supplements?</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lsf53j/what_are_your_thoughts_on_nail_supplements/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1lsf1sm</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>Summer set</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsf1sm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1lsemtu</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>Are these bad? Just got them done.</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kljh6th73bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1lseepl</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Durable nail options?</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78a9eg2u53bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1lseboc</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Chrome Bois</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qkdahf3753bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1lse3tt</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>Weeknd nails ahead of his concert tonight.</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lse3tt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1lse1wk</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>I’m obsessed and a little impressed with myself</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lse1wk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1lsdy6u</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Fourth of July Mani</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsdy6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1lsdvue</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Don’t just say it, scream it</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ba6oqlmp13bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1lsdrf0</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Weekend nails done</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1rktvytp03bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1ls9vl2</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Can someone tell me what’s happening with the top coat?</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hgcccoy42bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1lsdis4</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Some pretty summer nails</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsdis4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1lsdioi</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>are these too sharp?😅😅</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsdioi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1lsdb3s</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>Butterfly wings?</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wwzc047x2bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1lscrcn</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>3d “dew drops” are redirection tools for my clients who stim or pick at their cuticles. bonus, they look really cool :)</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7lsgl5xs2bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1lscqta</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Greec(e)y Vibes</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ezhfhdtss2bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1lsci9o</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Wdyt??</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsci9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1lscgfj</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Perfect length for comfort and chic</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lscgfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1lsc98x</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>My nail tech is a magician. What do we think?</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsc98x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1lsc320</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>stupid easy first try</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsc320</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1lsb9wy</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Tips for regular manis?</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crvcxqoyg2bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1lsb5jf</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>DIY Cinderella set!! Kinda nailed my non-dominant this time</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ratgqjtof2bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1lsb459</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>my mom's first time doing nails</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsb459</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1lsas4r</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Nail Biter Getting Nails Done</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsas4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1lsa032</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>blueberry lemonade nails 🫐🍋</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsa032</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1ls97u7</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Happy Fourth of July!</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xgqbn7uzy1bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1ls966e</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>first time to do my nails with arts isnt ok ?</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkc79p8ky1bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1ls9658</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>Exploring new colours since I usually gravitate to pinks!</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oemdffzjy1bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1ls8f3u</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>1 month nails progress</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls8f3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1lsu2ji</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>🍓 Strawberry nails for my bday week! 🍓</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsu2ji</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1lssybc</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Has anyone used the Brother P-touch Label Maker PT-H110 to label your swatch sticks?</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxcr0jzmp6bf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1lsrhca</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>Dupe requests for this dusty pink I mixed</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsrhca</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1lsqvy4</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>💙 Mood Ring 💚</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsqvy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1lsqspw</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>4th of July 🇺🇸</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsqspw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1lsqk6x</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>An attempt at the Carved Candle look 🌈🕯️</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsqk6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1lsq385</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>This might be the most interesting polish I own</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsq385</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1lspmrt</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Random question</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lspmrt/random_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1lsplat</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>How to remove gel manicure I got done today  😭</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsplat</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1lspf11</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>my mildewy queen</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lspf11</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1lsp99m</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>✨🌸Flower Child + Cohesion 🌸✨</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsp99m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1lsp8v5</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>I’m late but here’s my June roundup 🌈</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsp8v5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1lsp8aa</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsp8aa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1lsp6qw</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>Has anyone used this?</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1qbg349n5bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1lsnhf1</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>Purple Blade of the Frontiers??</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1rmc7jf75bf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1lsn31g</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>Anna Sui exhibit at the Phoenix Art Museum has a nail polish/cosmetic section and I’m enthralled</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bekedrjt35bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1lsmuga</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>if you’re on the fence about buying Renaissance by Patty Lopes here’s your sign!</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/11f0rtjq15bf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1lsmout</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>First Lurid order</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsmout</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1lsj1i0</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>Birthday Brat</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0weoz5n664bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1lsmd3v</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>Watercolor nails</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsmd3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1lslydx</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>Problems with CND Vinylux?</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpnjsbzyt4bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1lslsf4</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>Matching my hydrangea</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7amatia8s4bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1lskz3x</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>Indie versions of this shade?</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8n1ifujsl4bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1lsktld</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>Havasupai Falls</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ma7a1exhk4bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1lskpyl</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>Red jelly comparisons?</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lskpyl/red_jelly_comparisons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1lsknza</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>My First Lurid Order Arrived!! feat cardboard queen👸 💅</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ewqts818j4bf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1lsjl31</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>Cuticle oil pens</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsjl31</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1lsj6ub</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>White polishes similar to Mooncat's 'Head in the Clouds'?</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lsj6ub/white_polishes_similar_to_mooncats_head_in_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1lsiu7a</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>Root of All Evil - this color is straight out of a spellbook!</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsiu7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>1lsiryx</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>Yellow isn’t my color, but it’s my favorite, and don’t we all need a little joy, unflattering or not?</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsiryx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr">
+        <is>
+          <t>1lsiggz</t>
+        </is>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - A Pain in the Astroid 2.0</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsiggz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr">
+        <is>
+          <t>1lsi61z</t>
+        </is>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>Gratitude post - Stolen Kiss!</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ahqfmrz5z3bf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr">
+        <is>
+          <t>1lshu9c</t>
+        </is>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>Should I cut my nails?</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bh412r7iw3bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr">
+        <is>
+          <t>1lshts6</t>
+        </is>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>A blue shade like this?</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upt7k2rew3bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr">
+        <is>
+          <t>1lshq8e</t>
+        </is>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>My Fourth of July nails! I wanted to experiment with a thermal design that transitions between red/white stripes and blue</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lshq8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr">
+        <is>
+          <t>1lsh989</t>
+        </is>
+      </c>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>Unmagnetized swatches</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lsh989/unmagnetized_swatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr">
+        <is>
+          <t>1lsh3yk</t>
+        </is>
+      </c>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>Death Valley Nails - Stay a While + flakies</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqnmufusq3bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr">
+        <is>
+          <t>1lsgo36</t>
+        </is>
+      </c>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>Independence Day!</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsgo36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1490">
+      <c r="A1490" t="inlineStr">
+        <is>
+          <t>1lsgkdi</t>
+        </is>
+      </c>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>OPI Manicure</t>
+        </is>
+      </c>
+      <c r="C1490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7v5g2elm3bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1491">
+      <c r="A1491" t="inlineStr">
+        <is>
+          <t>1lsg5ei</t>
+        </is>
+      </c>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>MEATBALL</t>
+        </is>
+      </c>
+      <c r="C1491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsg5ei</t>
+        </is>
+      </c>
+    </row>
+    <row r="1492">
+      <c r="A1492" t="inlineStr">
+        <is>
+          <t>1lsg25z</t>
+        </is>
+      </c>
+      <c r="B1492" t="inlineStr">
+        <is>
+          <t>This one is SO hard to photograph... Whispering Waves by Psyche Minerals 🌊🩷🌸</t>
+        </is>
+      </c>
+      <c r="C1492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsg25z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1493">
+      <c r="A1493" t="inlineStr">
+        <is>
+          <t>1lsfdtp</t>
+        </is>
+      </c>
+      <c r="B1493" t="inlineStr">
+        <is>
+          <t>Cosmic Energy🪐🩵</t>
+        </is>
+      </c>
+      <c r="C1493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsfdtp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1494">
+      <c r="A1494" t="inlineStr">
+        <is>
+          <t>1lsfa0f</t>
+        </is>
+      </c>
+      <c r="B1494" t="inlineStr">
+        <is>
+          <t>This polish 🤯</t>
+        </is>
+      </c>
+      <c r="C1494" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2zsmjcefc3bf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1495">
+      <c r="A1495" t="inlineStr">
+        <is>
+          <t>1lsf631</t>
+        </is>
+      </c>
+      <c r="B1495" t="inlineStr">
+        <is>
+          <t>Pucker up 💋</t>
+        </is>
+      </c>
+      <c r="C1495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsf631</t>
+        </is>
+      </c>
+    </row>
+    <row r="1496">
+      <c r="A1496" t="inlineStr">
+        <is>
+          <t>1lsevef</t>
+        </is>
+      </c>
+      <c r="B1496" t="inlineStr">
+        <is>
+          <t>Living my best Barbie life</t>
+        </is>
+      </c>
+      <c r="C1496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsevef</t>
+        </is>
+      </c>
+    </row>
+    <row r="1497">
+      <c r="A1497" t="inlineStr">
+        <is>
+          <t>1lsenl1</t>
+        </is>
+      </c>
+      <c r="B1497" t="inlineStr">
+        <is>
+          <t>my first full gradient 🤍💜</t>
+        </is>
+      </c>
+      <c r="C1497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1ckam0n73bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1498">
+      <c r="A1498" t="inlineStr">
+        <is>
+          <t>1lsee3j</t>
+        </is>
+      </c>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t>Better Belize It 🩵</t>
+        </is>
+      </c>
+      <c r="C1498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsee3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1499">
+      <c r="A1499" t="inlineStr">
+        <is>
+          <t>1lsdjuv</t>
+        </is>
+      </c>
+      <c r="B1499" t="inlineStr">
+        <is>
+          <t>LA Colors - Glitter Vibes Jelly Bella</t>
+        </is>
+      </c>
+      <c r="C1499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsdjuv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1500">
+      <c r="A1500" t="inlineStr">
+        <is>
+          <t>1lsdd42</t>
+        </is>
+      </c>
+      <c r="B1500" t="inlineStr">
+        <is>
+          <t>Holo Taco- Vitamin Glow</t>
+        </is>
+      </c>
+      <c r="C1500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hs5j40umx2bf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1501">
+      <c r="A1501" t="inlineStr">
+        <is>
+          <t>1lscwzl</t>
+        </is>
+      </c>
+      <c r="B1501" t="inlineStr">
+        <is>
+          <t>FINALLY have my nails back after a year!</t>
+        </is>
+      </c>
+      <c r="C1501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oh0pz2t5u2bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1502">
+      <c r="A1502" t="inlineStr">
+        <is>
+          <t>1lscvgk</t>
+        </is>
+      </c>
+      <c r="B1502" t="inlineStr">
+        <is>
+          <t>4th of July Fireworks</t>
+        </is>
+      </c>
+      <c r="C1502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lscvgk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1503">
+      <c r="A1503" t="inlineStr">
+        <is>
+          <t>1lsclw0</t>
+        </is>
+      </c>
+      <c r="B1503" t="inlineStr">
+        <is>
+          <t>Trying to stop nail biting-3 weeks into my polish journey !</t>
+        </is>
+      </c>
+      <c r="C1503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsclw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1504">
+      <c r="A1504" t="inlineStr">
+        <is>
+          <t>1lschdo</t>
+        </is>
+      </c>
+      <c r="B1504" t="inlineStr">
+        <is>
+          <t>💙🥚Togepi!🥚❤️</t>
+        </is>
+      </c>
+      <c r="C1504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lschdo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1505">
+      <c r="A1505" t="inlineStr">
+        <is>
+          <t>1lscanw</t>
+        </is>
+      </c>
+      <c r="B1505" t="inlineStr">
+        <is>
+          <t>Anyone ever tried the spiral design with non-gel magnetics? Would it even work?</t>
+        </is>
+      </c>
+      <c r="C1505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhbea0w6p2bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1506">
+      <c r="A1506" t="inlineStr">
+        <is>
+          <t>1lsc9g6</t>
+        </is>
+      </c>
+      <c r="B1506" t="inlineStr">
+        <is>
+          <t>Gotta love the glow!</t>
+        </is>
+      </c>
+      <c r="C1506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/797gnrlto2bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1507">
+      <c r="A1507" t="inlineStr">
+        <is>
+          <t>1lsc4uw</t>
+        </is>
+      </c>
+      <c r="B1507" t="inlineStr">
+        <is>
+          <t>A patient told me they look like the inside of a seashell 🐚</t>
+        </is>
+      </c>
+      <c r="C1507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vrsx0qun2bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1508">
+      <c r="A1508" t="inlineStr">
+        <is>
+          <t>1lsbrxb</t>
+        </is>
+      </c>
+      <c r="B1508" t="inlineStr">
+        <is>
+          <t>Flower Child</t>
+        </is>
+      </c>
+      <c r="C1508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsbrxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1509">
+      <c r="A1509" t="inlineStr">
+        <is>
+          <t>1lsarrg</t>
+        </is>
+      </c>
+      <c r="B1509" t="inlineStr">
+        <is>
+          <t>Phases of my thermal patriotic mood- mani</t>
+        </is>
+      </c>
+      <c r="C1509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsarrg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1510">
+      <c r="A1510" t="inlineStr">
+        <is>
+          <t>1lsaiht</t>
+        </is>
+      </c>
+      <c r="B1510" t="inlineStr">
+        <is>
+          <t>Trying on my engagement ring and wedding band with Mooncat’s Moonfairy</t>
+        </is>
+      </c>
+      <c r="C1510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsaiht</t>
+        </is>
+      </c>
+    </row>
+    <row r="1511">
+      <c r="A1511" t="inlineStr">
+        <is>
+          <t>1lsahoi</t>
+        </is>
+      </c>
+      <c r="B1511" t="inlineStr">
+        <is>
+          <t>Anyone else (dis)illusioned by Alice?</t>
+        </is>
+      </c>
+      <c r="C1511" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1cqadrlx82bf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1512">
+      <c r="A1512" t="inlineStr">
+        <is>
+          <t>1ls95ey</t>
+        </is>
+      </c>
+      <c r="B1512" t="inlineStr">
+        <is>
+          <t>BKL June drop - promised 💕</t>
+        </is>
+      </c>
+      <c r="C1512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls95ey</t>
+        </is>
+      </c>
+    </row>
+    <row r="1513">
+      <c r="A1513" t="inlineStr">
+        <is>
+          <t>1ls7mxf</t>
+        </is>
+      </c>
+      <c r="B1513" t="inlineStr">
+        <is>
+          <t>First Post + Damaged Nail Recovery = Surprisingly Long-Lasting Mani!</t>
+        </is>
+      </c>
+      <c r="C1513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iudobhcsi1bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1514">
+      <c r="A1514" t="inlineStr">
+        <is>
+          <t>1ls7jmf</t>
+        </is>
+      </c>
+      <c r="B1514" t="inlineStr">
+        <is>
+          <t>Swatching seawinkle to see if I need a backup bottle from rewind 🤔</t>
+        </is>
+      </c>
+      <c r="C1514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls7jmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1515">
+      <c r="A1515" t="inlineStr">
+        <is>
+          <t>1ls5zs2</t>
+        </is>
+      </c>
+      <c r="B1515" t="inlineStr">
+        <is>
+          <t>By Vanessa Molina Easter Egg: reality vs swatch photos</t>
+        </is>
+      </c>
+      <c r="C1515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls5zs2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1516">
+      <c r="A1516" t="inlineStr">
+        <is>
+          <t>1lsllny</t>
+        </is>
+      </c>
+      <c r="B1516" t="inlineStr">
+        <is>
+          <t>Holographic butterfly  💿🦋 (beginner so it’s kinda messy lol)</t>
+        </is>
+      </c>
+      <c r="C1516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldy1o921r4bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1517">
+      <c r="A1517" t="inlineStr">
+        <is>
+          <t>1lsoz1w</t>
+        </is>
+      </c>
+      <c r="B1517" t="inlineStr">
+        <is>
+          <t>Loving the fruit basket nails lately!</t>
+        </is>
+      </c>
+      <c r="C1517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsoz1w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1518">
+      <c r="A1518" t="inlineStr">
+        <is>
+          <t>1lsrx16</t>
+        </is>
+      </c>
+      <c r="B1518" t="inlineStr">
+        <is>
+          <t>Little flowers to brighten your day 🌸</t>
+        </is>
+      </c>
+      <c r="C1518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3hezxzre6bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1519">
+      <c r="A1519" t="inlineStr">
+        <is>
+          <t>1lss140</t>
+        </is>
+      </c>
+      <c r="B1519" t="inlineStr">
+        <is>
+          <t>Upside down nail art?</t>
+        </is>
+      </c>
+      <c r="C1519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lss140/upside_down_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1520">
+      <c r="A1520" t="inlineStr">
+        <is>
+          <t>1lsrwp3</t>
+        </is>
+      </c>
+      <c r="B1520" t="inlineStr">
+        <is>
+          <t>Nail art ideas!</t>
+        </is>
+      </c>
+      <c r="C1520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kugp7jwoe6bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1521">
+      <c r="A1521" t="inlineStr">
+        <is>
+          <t>1lsr1xg</t>
+        </is>
+      </c>
+      <c r="B1521" t="inlineStr">
+        <is>
+          <t>Need a Nail salon suggestion for Silverdale WA.</t>
+        </is>
+      </c>
+      <c r="C1521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lsr1xg/need_a_nail_salon_suggestion_for_silverdale_wa/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1522">
+      <c r="A1522" t="inlineStr">
+        <is>
+          <t>1lsp07j</t>
+        </is>
+      </c>
+      <c r="B1522" t="inlineStr">
+        <is>
+          <t>I'm not sure if they're pretty or not at all, what do you think?</t>
+        </is>
+      </c>
+      <c r="C1522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgag7pskl5bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1523">
+      <c r="A1523" t="inlineStr">
+        <is>
+          <t>1lsoydl</t>
+        </is>
+      </c>
+      <c r="B1523" t="inlineStr">
+        <is>
+          <t>Alguien fan del negro?</t>
+        </is>
+      </c>
+      <c r="C1523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8hr5gg1l5bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1524">
+      <c r="A1524" t="inlineStr">
+        <is>
+          <t>1lsoxmr</t>
+        </is>
+      </c>
+      <c r="B1524" t="inlineStr">
+        <is>
+          <t>Estás de hoy 💅</t>
+        </is>
+      </c>
+      <c r="C1524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37xcnh1uk5bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1525">
+      <c r="A1525" t="inlineStr">
+        <is>
+          <t>1lsouks</t>
+        </is>
+      </c>
+      <c r="B1525" t="inlineStr">
+        <is>
+          <t>Just bought these colors for summer! So beautiful 🥰</t>
+        </is>
+      </c>
+      <c r="C1525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsouks</t>
+        </is>
+      </c>
+    </row>
+    <row r="1526">
+      <c r="A1526" t="inlineStr">
+        <is>
+          <t>1lsmgu7</t>
+        </is>
+      </c>
+      <c r="B1526" t="inlineStr">
+        <is>
+          <t>Progression</t>
+        </is>
+      </c>
+      <c r="C1526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ow3x12fy4bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1527">
+      <c r="A1527" t="inlineStr">
+        <is>
+          <t>1lsmd73</t>
+        </is>
+      </c>
+      <c r="B1527" t="inlineStr">
+        <is>
+          <t>🌊Ocean theme nail(on a chef hand)💙</t>
+        </is>
+      </c>
+      <c r="C1527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsmd73</t>
+        </is>
+      </c>
+    </row>
+    <row r="1528">
+      <c r="A1528" t="inlineStr">
+        <is>
+          <t>1lsl5od</t>
+        </is>
+      </c>
+      <c r="B1528" t="inlineStr">
+        <is>
+          <t>Beachy Nails 🏝️</t>
+        </is>
+      </c>
+      <c r="C1528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsl5od</t>
+        </is>
+      </c>
+    </row>
+    <row r="1529">
+      <c r="A1529" t="inlineStr">
+        <is>
+          <t>1lsjrq9</t>
+        </is>
+      </c>
+      <c r="B1529" t="inlineStr">
+        <is>
+          <t>My sister made me this beautiful design @renovarte_studio</t>
+        </is>
+      </c>
+      <c r="C1529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsjrq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1530">
+      <c r="A1530" t="inlineStr">
+        <is>
+          <t>1lsj3wc</t>
+        </is>
+      </c>
+      <c r="B1530" t="inlineStr">
+        <is>
+          <t>Wedding Nail Inspo</t>
+        </is>
+      </c>
+      <c r="C1530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lsj3wc/wedding_nail_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1531">
+      <c r="A1531" t="inlineStr">
+        <is>
+          <t>1lsia60</t>
+        </is>
+      </c>
+      <c r="B1531" t="inlineStr">
+        <is>
+          <t>When can i take a break?</t>
+        </is>
+      </c>
+      <c r="C1531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lsia60/when_can_i_take_a_break/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1532">
+      <c r="A1532" t="inlineStr">
+        <is>
+          <t>1lshjyu</t>
+        </is>
+      </c>
+      <c r="B1532" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C1532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kyzcwd59u3bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1533">
+      <c r="A1533" t="inlineStr">
+        <is>
+          <t>1lsh0v4</t>
+        </is>
+      </c>
+      <c r="B1533" t="inlineStr">
+        <is>
+          <t>First time doing gel nails after a few years! How did I do?</t>
+        </is>
+      </c>
+      <c r="C1533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6l05dzr4q3bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1534">
+      <c r="A1534" t="inlineStr">
+        <is>
+          <t>1lsglob</t>
+        </is>
+      </c>
+      <c r="B1534" t="inlineStr">
+        <is>
+          <t>Can you guess the movie that inspires this set ~? 🐟 🐠 🎣</t>
+        </is>
+      </c>
+      <c r="C1534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsglob</t>
+        </is>
+      </c>
+    </row>
+    <row r="1535">
+      <c r="A1535" t="inlineStr">
+        <is>
+          <t>1lsfaf8</t>
+        </is>
+      </c>
+      <c r="B1535" t="inlineStr">
+        <is>
+          <t>Glamrdip + gel stamp</t>
+        </is>
+      </c>
+      <c r="C1535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0tbm49gc3bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1536">
+      <c r="A1536" t="inlineStr">
+        <is>
+          <t>1lsfa0e</t>
+        </is>
+      </c>
+      <c r="B1536" t="inlineStr">
+        <is>
+          <t>love the lil tooth on this set :,)</t>
+        </is>
+      </c>
+      <c r="C1536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsfa0e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1537">
+      <c r="A1537" t="inlineStr">
+        <is>
+          <t>1lsf0wa</t>
+        </is>
+      </c>
+      <c r="B1537" t="inlineStr">
+        <is>
+          <t>Summer set</t>
+        </is>
+      </c>
+      <c r="C1537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsf0wa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1538">
+      <c r="A1538" t="inlineStr">
+        <is>
+          <t>1lsavsn</t>
+        </is>
+      </c>
+      <c r="B1538" t="inlineStr">
+        <is>
+          <t>Summer fruits</t>
+        </is>
+      </c>
+      <c r="C1538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lsavsn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1539">
+      <c r="A1539" t="inlineStr">
+        <is>
+          <t>1ls68zu</t>
+        </is>
+      </c>
+      <c r="B1539" t="inlineStr">
+        <is>
+          <t>Italian summer vibes💙💛🤍🍋</t>
+        </is>
+      </c>
+      <c r="C1539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5iv5eod521bf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1540">
+      <c r="A1540" t="inlineStr">
+        <is>
+          <t>1ls5to2</t>
+        </is>
+      </c>
+      <c r="B1540" t="inlineStr">
+        <is>
+          <t>Neon watercolor</t>
+        </is>
+      </c>
+      <c r="C1540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ls5to2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>